<commit_message>
add comments to properties
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376333EE-65AB-E549-8A9D-A844BB8CB522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE474518-9F78-CE44-95D9-10D721C974DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="55200" windowHeight="22640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="369">
   <si>
     <t>name</t>
   </si>
@@ -739,18 +739,6 @@
     <t>linkToAudio</t>
   </si>
   <si>
-    <t>linked Audio</t>
-  </si>
-  <si>
-    <t>Verknüpftes Audio</t>
-  </si>
-  <si>
-    <t>Audio lié</t>
-  </si>
-  <si>
-    <t>Audio correlato</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:audio</t>
   </si>
   <si>
@@ -781,18 +769,6 @@
     <t>linkToBookEdition</t>
   </si>
   <si>
-    <t>linked Edition</t>
-  </si>
-  <si>
-    <t>verlinkte Ausgabe</t>
-  </si>
-  <si>
-    <t>Edition liée</t>
-  </si>
-  <si>
-    <t>Edizione correlata</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:bookEdition</t>
   </si>
   <si>
@@ -802,18 +778,6 @@
     <t>linkToCharacter</t>
   </si>
   <si>
-    <t>linked Character(s)</t>
-  </si>
-  <si>
-    <t>verlinkte(r) Charakter(e)</t>
-  </si>
-  <si>
-    <t>Personnage(s) lié(s)</t>
-  </si>
-  <si>
-    <t>Personaggio/i correlato/i</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:character, crm:P11_had_participant</t>
   </si>
   <si>
@@ -853,18 +817,6 @@
     <t>linkToEvent</t>
   </si>
   <si>
-    <t>linked Event</t>
-  </si>
-  <si>
-    <t>verlinktes Ereignis</t>
-  </si>
-  <si>
-    <t>Evénement lié</t>
-  </si>
-  <si>
-    <t>Evento correlato</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:event</t>
   </si>
   <si>
@@ -874,18 +826,6 @@
     <t>linkToImage</t>
   </si>
   <si>
-    <t>linked Image</t>
-  </si>
-  <si>
-    <t>verlinktes Bild</t>
-  </si>
-  <si>
-    <t>Image liée</t>
-  </si>
-  <si>
-    <t>Immagine collegata</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:image</t>
   </si>
   <si>
@@ -916,18 +856,6 @@
     <t>linkToVideo</t>
   </si>
   <si>
-    <t>linked Video</t>
-  </si>
-  <si>
-    <t>verlinktes Video</t>
-  </si>
-  <si>
-    <t>Vidéo liée</t>
-  </si>
-  <si>
-    <t>Video correlato</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:video</t>
   </si>
   <si>
@@ -937,18 +865,6 @@
     <t>linkToBookCover</t>
   </si>
   <si>
-    <t>linked Book Cover</t>
-  </si>
-  <si>
-    <t>verlinktes Einband</t>
-  </si>
-  <si>
-    <t>Couverture liée</t>
-  </si>
-  <si>
-    <t>Copertine correlata</t>
-  </si>
-  <si>
     <t>:BookCover</t>
   </si>
   <si>
@@ -962,18 +878,427 @@
   </si>
   <si>
     <t>Auteur·ice</t>
+  </si>
+  <si>
+    <t>Importance of the character in the story</t>
+  </si>
+  <si>
+    <t>Sequence number used for compound object</t>
+  </si>
+  <si>
+    <t>Time stamp</t>
+  </si>
+  <si>
+    <t>URL leading to an external page with more information</t>
+  </si>
+  <si>
+    <t>Is the event dangerous?</t>
+  </si>
+  <si>
+    <t>Belongs to following book</t>
+  </si>
+  <si>
+    <t>internal link to the Edition(s)</t>
+  </si>
+  <si>
+    <t>internal link to Character(s)</t>
+  </si>
+  <si>
+    <t>internal link to Event(s)</t>
+  </si>
+  <si>
+    <t>internal link to Image(s)</t>
+  </si>
+  <si>
+    <t>internal link to Location(s)</t>
+  </si>
+  <si>
+    <t>internal link to Video(s)</t>
+  </si>
+  <si>
+    <t>internal link to Book Cover(s)</t>
+  </si>
+  <si>
+    <t>internal link to Antagonist(s)</t>
+  </si>
+  <si>
+    <t>internal link to Protagonist(s)</t>
+  </si>
+  <si>
+    <t>Auteur ou créateur du fichier</t>
+  </si>
+  <si>
+    <t>Membres de la distribution qui apparaissent sur le média</t>
+  </si>
+  <si>
+    <t>Numéro du chapitre</t>
+  </si>
+  <si>
+    <t>Copyright du fichier média</t>
+  </si>
+  <si>
+    <t>Description de l'œuvre</t>
+  </si>
+  <si>
+    <t>Description alternative, faite pour fournir un exemple de valeur restreinte</t>
+  </si>
+  <si>
+    <t>Type d'événement, déterminé par une liste</t>
+  </si>
+  <si>
+    <t>Nom du fichier original</t>
+  </si>
+  <si>
+    <t>Taille du fichier en Mo</t>
+  </si>
+  <si>
+    <t>Texte en anglais</t>
+  </si>
+  <si>
+    <t>Nombre d'invités à l'événement</t>
+  </si>
+  <si>
+    <t>Identifiant unique</t>
+  </si>
+  <si>
+    <t>Licence d'utilisation du fichier média</t>
+  </si>
+  <si>
+    <t>Citation, telle qu'elle est écrite dans l'histoire originale</t>
+  </si>
+  <si>
+    <t>Importance du personnage dans l'histoire</t>
+  </si>
+  <si>
+    <t>Numéro de séquence utilisé pour l'objet composé</t>
+  </si>
+  <si>
+    <t>URL menant à une page externe contenant plus d'informations</t>
+  </si>
+  <si>
+    <t>L'événement est-il dangereux ?</t>
+  </si>
+  <si>
+    <t>Appartient au livre suivant</t>
+  </si>
+  <si>
+    <t>lien interne vers l'(les) édition(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers le(s) personnage(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Antagoniste(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Protagoniste(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Événement(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Image(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Lieu(x)</t>
+  </si>
+  <si>
+    <t>lien interne vers Vidéo(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Couverture(s) de livre</t>
+  </si>
+  <si>
+    <t>Lien vers le lieu sur le site de geonames</t>
+  </si>
+  <si>
+    <t>Mots-clés associés à l'enregistrement</t>
+  </si>
+  <si>
+    <t>internal link to Book Chapters</t>
+  </si>
+  <si>
+    <t>Edition</t>
+  </si>
+  <si>
+    <t>Character(s)</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Book Cover</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Ausgabe</t>
+  </si>
+  <si>
+    <t>Charakter(e)</t>
+  </si>
+  <si>
+    <t>Ereignis</t>
+  </si>
+  <si>
+    <t>Bild</t>
+  </si>
+  <si>
+    <t>Einband</t>
+  </si>
+  <si>
+    <t>Personnage(s)</t>
+  </si>
+  <si>
+    <t>Evénement(s)</t>
+  </si>
+  <si>
+    <t>Event(s)</t>
+  </si>
+  <si>
+    <t>Image(s)</t>
+  </si>
+  <si>
+    <t>Image(s) liée(s)</t>
+  </si>
+  <si>
+    <t>Vidéo</t>
+  </si>
+  <si>
+    <t>Couverture</t>
+  </si>
+  <si>
+    <t>Edizione</t>
+  </si>
+  <si>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>Immagine</t>
+  </si>
+  <si>
+    <t>Copertine</t>
+  </si>
+  <si>
+    <t>Personaggio/i</t>
+  </si>
+  <si>
+    <t>internal link to Audio</t>
+  </si>
+  <si>
+    <t>lien interne vers les Chapitres du livre</t>
+  </si>
+  <si>
+    <t>lien interne vers les fichiers Audio</t>
+  </si>
+  <si>
+    <t>Autor oder Urheber der Datei</t>
+  </si>
+  <si>
+    <t>Darsteller, die in den Medien erscheinen</t>
+  </si>
+  <si>
+    <t>Nummer des Kapitels</t>
+  </si>
+  <si>
+    <t>Urheberrecht der Mediendatei</t>
+  </si>
+  <si>
+    <t>Veröffentlichungsdatum</t>
+  </si>
+  <si>
+    <t>Alternative Beschreibung, um ein Beispiel für einen eingeschränkten Wert zu geben</t>
+  </si>
+  <si>
+    <t>Art der Veranstaltung, anhand einer Liste festgelegt</t>
+  </si>
+  <si>
+    <t>Name der Originaldatei</t>
+  </si>
+  <si>
+    <t>Dateigröße in MB</t>
+  </si>
+  <si>
+    <t>Text in englischer Sprache</t>
+  </si>
+  <si>
+    <t>Link zum Ort auf der Geonames-Website</t>
+  </si>
+  <si>
+    <t>Anzahl der Gäste der Veranstaltung</t>
+  </si>
+  <si>
+    <t>Eindeutige Kennung</t>
+  </si>
+  <si>
+    <t>Mit dem Datensatz verbundene Schlüsselwörter</t>
+  </si>
+  <si>
+    <t>Lizenz zur Nutzung der Mediendatei</t>
+  </si>
+  <si>
+    <t>Zitat, wie im Originaltext geschrieben</t>
+  </si>
+  <si>
+    <t>Bedeutung der Figur in der Geschichte</t>
+  </si>
+  <si>
+    <t>Sequenznummer für zusammengesetzte Objekte</t>
+  </si>
+  <si>
+    <t>URL zu einer externen Seite mit weiteren Informationen</t>
+  </si>
+  <si>
+    <t>Ist das Ereignis gefährlich?</t>
+  </si>
+  <si>
+    <t>Gehört zu folgendem Buch</t>
+  </si>
+  <si>
+    <t>Interner Link zu Audio</t>
+  </si>
+  <si>
+    <t>Interner Link zu Buchkapiteln</t>
+  </si>
+  <si>
+    <t>Interner Link zu den Ausgaben</t>
+  </si>
+  <si>
+    <t>Interner Link zu Figur(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Antagonist(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Protagonist(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Ereignis(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Bild(ern)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Ort(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Video(s)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Buchcover(s)</t>
+  </si>
+  <si>
+    <t>Autore o creatore del file</t>
+  </si>
+  <si>
+    <t>Cast dei membri che compaiono nel media</t>
+  </si>
+  <si>
+    <t>Copyright del file multimediale</t>
+  </si>
+  <si>
+    <t>Descrizione alternativa, fornita per fornire un esempio di valore limitato</t>
+  </si>
+  <si>
+    <t>Tipo di evento, determinato da un elenco</t>
+  </si>
+  <si>
+    <t>Nome del file originale</t>
+  </si>
+  <si>
+    <t>Dimensione del file in Mb</t>
+  </si>
+  <si>
+    <t>Testo in inglese</t>
+  </si>
+  <si>
+    <t>Link al luogo sul sito web geonames</t>
+  </si>
+  <si>
+    <t>Numero di ospiti all'evento</t>
+  </si>
+  <si>
+    <t>Identificatore univoco</t>
+  </si>
+  <si>
+    <t>Parole chiave associate alla scheda</t>
+  </si>
+  <si>
+    <t>Licenza d'uso del file multimediale</t>
+  </si>
+  <si>
+    <t>Citazione, come riportata nella storia originale</t>
+  </si>
+  <si>
+    <t>Importanza del personaggio nella storia</t>
+  </si>
+  <si>
+    <t>Numero di sequenza utilizzato per oggetti composti</t>
+  </si>
+  <si>
+    <t>Data e ora</t>
+  </si>
+  <si>
+    <t>URL che rimanda a una pagina esterna con ulteriori informazioni</t>
+  </si>
+  <si>
+    <t>L'evento è pericoloso?</t>
+  </si>
+  <si>
+    <t>Appartiene al seguente libro</t>
+  </si>
+  <si>
+    <t>link interno all'audio</t>
+  </si>
+  <si>
+    <t>link interno ai capitoli del libro</t>
+  </si>
+  <si>
+    <t>link interno all'edizione/alle edizioni</t>
+  </si>
+  <si>
+    <t>link interno a Personaggio/i</t>
+  </si>
+  <si>
+    <t>link interno a Antagonista/i</t>
+  </si>
+  <si>
+    <t>link interno a Protagonista/i</t>
+  </si>
+  <si>
+    <t>link interno a Evento/i</t>
+  </si>
+  <si>
+    <t>link interno a Immagine/i</t>
+  </si>
+  <si>
+    <t>link interno a Luogo/i</t>
+  </si>
+  <si>
+    <t>link interno a Video/i</t>
+  </si>
+  <si>
+    <t>link interno a Copertina/e del libro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1044,15 +1369,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,9 +1596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q916"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1282,12 +1608,12 @@
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.1640625" customWidth="1"/>
     <col min="5" max="5" width="32.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" customWidth="1"/>
+    <col min="8" max="8" width="77.83203125" customWidth="1"/>
+    <col min="9" max="9" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="63" customWidth="1"/>
     <col min="13" max="13" width="29.1640625" customWidth="1"/>
     <col min="14" max="14" width="11.5" customWidth="1"/>
@@ -1346,16 +1672,16 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1363,9 +1689,15 @@
       <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>338</v>
+      </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1395,6 +1727,15 @@
       <c r="G3" t="s">
         <v>25</v>
       </c>
+      <c r="H3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I3" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" t="s">
+        <v>339</v>
+      </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
       </c>
@@ -1423,6 +1764,15 @@
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>308</v>
+      </c>
+      <c r="I4" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>34</v>
@@ -1453,6 +1803,15 @@
       </c>
       <c r="G5" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>41</v>
@@ -1485,6 +1844,15 @@
       <c r="G6" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="H6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I6" t="s">
+        <v>253</v>
+      </c>
+      <c r="J6" t="s">
+        <v>340</v>
+      </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1516,6 +1884,15 @@
       <c r="G7" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="H7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
       <c r="L7" s="4" t="s">
         <v>56</v>
       </c>
@@ -1546,8 +1923,15 @@
       <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="L8" s="4" t="s">
         <v>63</v>
       </c>
@@ -1579,8 +1963,15 @@
       <c r="G9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="H9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
       </c>
@@ -1612,7 +2003,15 @@
       <c r="G10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="H10" t="s">
+        <v>312</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="J10" t="s">
+        <v>342</v>
+      </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
       </c>
@@ -1645,8 +2044,15 @@
       <c r="G11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="J11" t="s">
+        <v>343</v>
+      </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
       </c>
@@ -1677,6 +2083,15 @@
       <c r="G12" t="s">
         <v>92</v>
       </c>
+      <c r="H12" t="s">
+        <v>314</v>
+      </c>
+      <c r="I12" t="s">
+        <v>258</v>
+      </c>
+      <c r="J12" t="s">
+        <v>344</v>
+      </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
       </c>
@@ -1706,6 +2121,15 @@
       <c r="G13" t="s">
         <v>100</v>
       </c>
+      <c r="H13" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J13" t="s">
+        <v>345</v>
+      </c>
       <c r="L13" s="4" t="s">
         <v>101</v>
       </c>
@@ -1735,7 +2159,15 @@
       <c r="G14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="H14" t="s">
+        <v>316</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J14" t="s">
+        <v>346</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>105</v>
       </c>
@@ -1767,6 +2199,15 @@
       <c r="G15" s="6" t="s">
         <v>113</v>
       </c>
+      <c r="H15" t="s">
+        <v>317</v>
+      </c>
+      <c r="I15" t="s">
+        <v>260</v>
+      </c>
+      <c r="J15" t="s">
+        <v>347</v>
+      </c>
       <c r="L15" s="4" t="s">
         <v>114</v>
       </c>
@@ -1795,6 +2236,15 @@
       </c>
       <c r="G16" s="4" t="s">
         <v>117</v>
+      </c>
+      <c r="H16" t="s">
+        <v>318</v>
+      </c>
+      <c r="I16" t="s">
+        <v>261</v>
+      </c>
+      <c r="J16" t="s">
+        <v>348</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>118</v>
@@ -1827,6 +2277,15 @@
       <c r="G17" t="s">
         <v>124</v>
       </c>
+      <c r="H17" t="s">
+        <v>319</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="J17" t="s">
+        <v>349</v>
+      </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
       </c>
@@ -1858,6 +2317,15 @@
       </c>
       <c r="G18" s="4" t="s">
         <v>132</v>
+      </c>
+      <c r="H18" t="s">
+        <v>320</v>
+      </c>
+      <c r="I18" t="s">
+        <v>262</v>
+      </c>
+      <c r="J18" t="s">
+        <v>350</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>133</v>
@@ -1893,7 +2361,15 @@
       <c r="G19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="H19" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
       <c r="L19" s="4" t="s">
         <v>86</v>
       </c>
@@ -1924,6 +2400,15 @@
       <c r="G20" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="H20" t="s">
+        <v>321</v>
+      </c>
+      <c r="I20" t="s">
+        <v>263</v>
+      </c>
+      <c r="J20" t="s">
+        <v>351</v>
+      </c>
       <c r="L20" s="4" t="s">
         <v>145</v>
       </c>
@@ -1951,7 +2436,18 @@
       <c r="E21" t="s">
         <v>150</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="H21" t="s">
+        <v>322</v>
+      </c>
+      <c r="I21" t="s">
+        <v>264</v>
+      </c>
+      <c r="J21" t="s">
+        <v>352</v>
+      </c>
       <c r="L21" s="4" t="s">
         <v>151</v>
       </c>
@@ -1983,8 +2479,18 @@
       <c r="E22" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="G22" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H22" t="s">
+        <v>323</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="J22" t="s">
+        <v>353</v>
+      </c>
       <c r="L22" s="4" t="s">
         <v>155</v>
       </c>
@@ -2013,7 +2519,18 @@
       <c r="E23" t="s">
         <v>160</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" t="s">
+        <v>159</v>
+      </c>
+      <c r="J23" t="s">
+        <v>354</v>
+      </c>
       <c r="L23" s="4" t="s">
         <v>161</v>
       </c>
@@ -2042,7 +2559,18 @@
       <c r="E24" t="s">
         <v>168</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I24" t="s">
+        <v>266</v>
+      </c>
+      <c r="J24" t="s">
+        <v>355</v>
+      </c>
       <c r="L24" s="4" t="s">
         <v>169</v>
       </c>
@@ -2069,7 +2597,18 @@
       <c r="E25" t="s">
         <v>175</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H25" t="s">
+        <v>325</v>
+      </c>
+      <c r="I25" t="s">
+        <v>267</v>
+      </c>
+      <c r="J25" t="s">
+        <v>356</v>
+      </c>
       <c r="L25" s="4" t="s">
         <v>176</v>
       </c>
@@ -2096,8 +2635,18 @@
       <c r="E26" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="G26" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="H26" t="s">
+        <v>326</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" t="s">
+        <v>357</v>
+      </c>
       <c r="L26" s="4" t="s">
         <v>184</v>
       </c>
@@ -2114,35 +2663,35 @@
       <c r="A27" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="J27" t="s">
+        <v>358</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C27" t="s">
+      <c r="M27" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="D27" t="s">
-        <v>190</v>
-      </c>
-      <c r="E27" t="s">
-        <v>191</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="H27" t="s">
-        <v>189</v>
-      </c>
-      <c r="I27" t="s">
-        <v>190</v>
-      </c>
-      <c r="J27" t="s">
-        <v>191</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>186</v>
@@ -2152,37 +2701,37 @@
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" t="s">
         <v>194</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="G28" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H28" t="s">
+        <v>328</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="J28" t="s">
+        <v>359</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C28" t="s">
+      <c r="M28" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="D28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E28" t="s">
-        <v>198</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H28" t="s">
-        <v>196</v>
-      </c>
-      <c r="I28" t="s">
-        <v>197</v>
-      </c>
-      <c r="J28" t="s">
-        <v>198</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>186</v>
@@ -2190,27 +2739,37 @@
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="I29" s="4"/>
+        <v>197</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H29" t="s">
+        <v>329</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="J29" t="s">
+        <v>360</v>
+      </c>
       <c r="L29" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>186</v>
@@ -2218,29 +2777,37 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+        <v>200</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>361</v>
+      </c>
       <c r="L30" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>186</v>
@@ -2250,26 +2817,37 @@
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C31" t="s">
-        <v>217</v>
-      </c>
-      <c r="D31" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>206</v>
       </c>
       <c r="E31" t="s">
-        <v>219</v>
-      </c>
-      <c r="G31" s="4"/>
+        <v>207</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H31" t="s">
+        <v>331</v>
+      </c>
+      <c r="I31" t="s">
+        <v>271</v>
+      </c>
+      <c r="J31" t="s">
+        <v>362</v>
+      </c>
       <c r="L31" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>186</v>
@@ -2277,26 +2855,37 @@
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D32" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E32" t="s">
-        <v>224</v>
-      </c>
-      <c r="G32" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" t="s">
+        <v>332</v>
+      </c>
+      <c r="I32" t="s">
+        <v>272</v>
+      </c>
+      <c r="J32" t="s">
+        <v>363</v>
+      </c>
       <c r="L32" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>186</v>
@@ -2304,25 +2893,37 @@
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>229</v>
+        <v>213</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H33" t="s">
+        <v>333</v>
+      </c>
+      <c r="I33" t="s">
+        <v>273</v>
+      </c>
+      <c r="J33" t="s">
+        <v>364</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>186</v>
@@ -2330,29 +2931,37 @@
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+        <v>216</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>365</v>
+      </c>
       <c r="L34" s="4" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>186</v>
@@ -2360,26 +2969,37 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>240</v>
+        <v>219</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="D35" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>223</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H35" t="s">
+        <v>335</v>
+      </c>
+      <c r="I35" t="s">
+        <v>275</v>
+      </c>
+      <c r="J35" t="s">
+        <v>366</v>
+      </c>
       <c r="L35" s="4" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>186</v>
@@ -2388,27 +3008,37 @@
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C36" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E36" t="s">
-        <v>250</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="H36" t="s">
+        <v>336</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="J36" t="s">
+        <v>367</v>
+      </c>
       <c r="L36" s="4" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>186</v>
@@ -2418,25 +3048,37 @@
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>257</v>
+        <v>229</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="H37" t="s">
+        <v>337</v>
+      </c>
+      <c r="I37" t="s">
+        <v>277</v>
+      </c>
+      <c r="J37" t="s">
+        <v>368</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
add comments to properties (#32)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielasubotic/Documents/GitHub/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{376333EE-65AB-E549-8A9D-A844BB8CB522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE474518-9F78-CE44-95D9-10D721C974DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="55200" windowHeight="22640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="369">
   <si>
     <t>name</t>
   </si>
@@ -739,18 +739,6 @@
     <t>linkToAudio</t>
   </si>
   <si>
-    <t>linked Audio</t>
-  </si>
-  <si>
-    <t>Verknüpftes Audio</t>
-  </si>
-  <si>
-    <t>Audio lié</t>
-  </si>
-  <si>
-    <t>Audio correlato</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:audio</t>
   </si>
   <si>
@@ -781,18 +769,6 @@
     <t>linkToBookEdition</t>
   </si>
   <si>
-    <t>linked Edition</t>
-  </si>
-  <si>
-    <t>verlinkte Ausgabe</t>
-  </si>
-  <si>
-    <t>Edition liée</t>
-  </si>
-  <si>
-    <t>Edizione correlata</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:bookEdition</t>
   </si>
   <si>
@@ -802,18 +778,6 @@
     <t>linkToCharacter</t>
   </si>
   <si>
-    <t>linked Character(s)</t>
-  </si>
-  <si>
-    <t>verlinkte(r) Charakter(e)</t>
-  </si>
-  <si>
-    <t>Personnage(s) lié(s)</t>
-  </si>
-  <si>
-    <t>Personaggio/i correlato/i</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:character, crm:P11_had_participant</t>
   </si>
   <si>
@@ -853,18 +817,6 @@
     <t>linkToEvent</t>
   </si>
   <si>
-    <t>linked Event</t>
-  </si>
-  <si>
-    <t>verlinktes Ereignis</t>
-  </si>
-  <si>
-    <t>Evénement lié</t>
-  </si>
-  <si>
-    <t>Evento correlato</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:event</t>
   </si>
   <si>
@@ -874,18 +826,6 @@
     <t>linkToImage</t>
   </si>
   <si>
-    <t>linked Image</t>
-  </si>
-  <si>
-    <t>verlinktes Bild</t>
-  </si>
-  <si>
-    <t>Image liée</t>
-  </si>
-  <si>
-    <t>Immagine collegata</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:image</t>
   </si>
   <si>
@@ -916,18 +856,6 @@
     <t>linkToVideo</t>
   </si>
   <si>
-    <t>linked Video</t>
-  </si>
-  <si>
-    <t>verlinktes Video</t>
-  </si>
-  <si>
-    <t>Vidéo liée</t>
-  </si>
-  <si>
-    <t>Video correlato</t>
-  </si>
-  <si>
     <t>hasLinkTo, schema:video</t>
   </si>
   <si>
@@ -937,18 +865,6 @@
     <t>linkToBookCover</t>
   </si>
   <si>
-    <t>linked Book Cover</t>
-  </si>
-  <si>
-    <t>verlinktes Einband</t>
-  </si>
-  <si>
-    <t>Couverture liée</t>
-  </si>
-  <si>
-    <t>Copertine correlata</t>
-  </si>
-  <si>
     <t>:BookCover</t>
   </si>
   <si>
@@ -962,18 +878,427 @@
   </si>
   <si>
     <t>Auteur·ice</t>
+  </si>
+  <si>
+    <t>Importance of the character in the story</t>
+  </si>
+  <si>
+    <t>Sequence number used for compound object</t>
+  </si>
+  <si>
+    <t>Time stamp</t>
+  </si>
+  <si>
+    <t>URL leading to an external page with more information</t>
+  </si>
+  <si>
+    <t>Is the event dangerous?</t>
+  </si>
+  <si>
+    <t>Belongs to following book</t>
+  </si>
+  <si>
+    <t>internal link to the Edition(s)</t>
+  </si>
+  <si>
+    <t>internal link to Character(s)</t>
+  </si>
+  <si>
+    <t>internal link to Event(s)</t>
+  </si>
+  <si>
+    <t>internal link to Image(s)</t>
+  </si>
+  <si>
+    <t>internal link to Location(s)</t>
+  </si>
+  <si>
+    <t>internal link to Video(s)</t>
+  </si>
+  <si>
+    <t>internal link to Book Cover(s)</t>
+  </si>
+  <si>
+    <t>internal link to Antagonist(s)</t>
+  </si>
+  <si>
+    <t>internal link to Protagonist(s)</t>
+  </si>
+  <si>
+    <t>Auteur ou créateur du fichier</t>
+  </si>
+  <si>
+    <t>Membres de la distribution qui apparaissent sur le média</t>
+  </si>
+  <si>
+    <t>Numéro du chapitre</t>
+  </si>
+  <si>
+    <t>Copyright du fichier média</t>
+  </si>
+  <si>
+    <t>Description de l'œuvre</t>
+  </si>
+  <si>
+    <t>Description alternative, faite pour fournir un exemple de valeur restreinte</t>
+  </si>
+  <si>
+    <t>Type d'événement, déterminé par une liste</t>
+  </si>
+  <si>
+    <t>Nom du fichier original</t>
+  </si>
+  <si>
+    <t>Taille du fichier en Mo</t>
+  </si>
+  <si>
+    <t>Texte en anglais</t>
+  </si>
+  <si>
+    <t>Nombre d'invités à l'événement</t>
+  </si>
+  <si>
+    <t>Identifiant unique</t>
+  </si>
+  <si>
+    <t>Licence d'utilisation du fichier média</t>
+  </si>
+  <si>
+    <t>Citation, telle qu'elle est écrite dans l'histoire originale</t>
+  </si>
+  <si>
+    <t>Importance du personnage dans l'histoire</t>
+  </si>
+  <si>
+    <t>Numéro de séquence utilisé pour l'objet composé</t>
+  </si>
+  <si>
+    <t>URL menant à une page externe contenant plus d'informations</t>
+  </si>
+  <si>
+    <t>L'événement est-il dangereux ?</t>
+  </si>
+  <si>
+    <t>Appartient au livre suivant</t>
+  </si>
+  <si>
+    <t>lien interne vers l'(les) édition(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers le(s) personnage(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Antagoniste(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Protagoniste(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Événement(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Image(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Lieu(x)</t>
+  </si>
+  <si>
+    <t>lien interne vers Vidéo(s)</t>
+  </si>
+  <si>
+    <t>lien interne vers Couverture(s) de livre</t>
+  </si>
+  <si>
+    <t>Lien vers le lieu sur le site de geonames</t>
+  </si>
+  <si>
+    <t>Mots-clés associés à l'enregistrement</t>
+  </si>
+  <si>
+    <t>internal link to Book Chapters</t>
+  </si>
+  <si>
+    <t>Edition</t>
+  </si>
+  <si>
+    <t>Character(s)</t>
+  </si>
+  <si>
+    <t>Video</t>
+  </si>
+  <si>
+    <t>Book Cover</t>
+  </si>
+  <si>
+    <t>Audio</t>
+  </si>
+  <si>
+    <t>Ausgabe</t>
+  </si>
+  <si>
+    <t>Charakter(e)</t>
+  </si>
+  <si>
+    <t>Ereignis</t>
+  </si>
+  <si>
+    <t>Bild</t>
+  </si>
+  <si>
+    <t>Einband</t>
+  </si>
+  <si>
+    <t>Personnage(s)</t>
+  </si>
+  <si>
+    <t>Evénement(s)</t>
+  </si>
+  <si>
+    <t>Event(s)</t>
+  </si>
+  <si>
+    <t>Image(s)</t>
+  </si>
+  <si>
+    <t>Image(s) liée(s)</t>
+  </si>
+  <si>
+    <t>Vidéo</t>
+  </si>
+  <si>
+    <t>Couverture</t>
+  </si>
+  <si>
+    <t>Edizione</t>
+  </si>
+  <si>
+    <t>Evento</t>
+  </si>
+  <si>
+    <t>Immagine</t>
+  </si>
+  <si>
+    <t>Copertine</t>
+  </si>
+  <si>
+    <t>Personaggio/i</t>
+  </si>
+  <si>
+    <t>internal link to Audio</t>
+  </si>
+  <si>
+    <t>lien interne vers les Chapitres du livre</t>
+  </si>
+  <si>
+    <t>lien interne vers les fichiers Audio</t>
+  </si>
+  <si>
+    <t>Autor oder Urheber der Datei</t>
+  </si>
+  <si>
+    <t>Darsteller, die in den Medien erscheinen</t>
+  </si>
+  <si>
+    <t>Nummer des Kapitels</t>
+  </si>
+  <si>
+    <t>Urheberrecht der Mediendatei</t>
+  </si>
+  <si>
+    <t>Veröffentlichungsdatum</t>
+  </si>
+  <si>
+    <t>Alternative Beschreibung, um ein Beispiel für einen eingeschränkten Wert zu geben</t>
+  </si>
+  <si>
+    <t>Art der Veranstaltung, anhand einer Liste festgelegt</t>
+  </si>
+  <si>
+    <t>Name der Originaldatei</t>
+  </si>
+  <si>
+    <t>Dateigröße in MB</t>
+  </si>
+  <si>
+    <t>Text in englischer Sprache</t>
+  </si>
+  <si>
+    <t>Link zum Ort auf der Geonames-Website</t>
+  </si>
+  <si>
+    <t>Anzahl der Gäste der Veranstaltung</t>
+  </si>
+  <si>
+    <t>Eindeutige Kennung</t>
+  </si>
+  <si>
+    <t>Mit dem Datensatz verbundene Schlüsselwörter</t>
+  </si>
+  <si>
+    <t>Lizenz zur Nutzung der Mediendatei</t>
+  </si>
+  <si>
+    <t>Zitat, wie im Originaltext geschrieben</t>
+  </si>
+  <si>
+    <t>Bedeutung der Figur in der Geschichte</t>
+  </si>
+  <si>
+    <t>Sequenznummer für zusammengesetzte Objekte</t>
+  </si>
+  <si>
+    <t>URL zu einer externen Seite mit weiteren Informationen</t>
+  </si>
+  <si>
+    <t>Ist das Ereignis gefährlich?</t>
+  </si>
+  <si>
+    <t>Gehört zu folgendem Buch</t>
+  </si>
+  <si>
+    <t>Interner Link zu Audio</t>
+  </si>
+  <si>
+    <t>Interner Link zu Buchkapiteln</t>
+  </si>
+  <si>
+    <t>Interner Link zu den Ausgaben</t>
+  </si>
+  <si>
+    <t>Interner Link zu Figur(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Antagonist(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Protagonist(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Ereignis(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Bild(ern)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Ort(en)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Video(s)</t>
+  </si>
+  <si>
+    <t>Interner Link zu Buchcover(s)</t>
+  </si>
+  <si>
+    <t>Autore o creatore del file</t>
+  </si>
+  <si>
+    <t>Cast dei membri che compaiono nel media</t>
+  </si>
+  <si>
+    <t>Copyright del file multimediale</t>
+  </si>
+  <si>
+    <t>Descrizione alternativa, fornita per fornire un esempio di valore limitato</t>
+  </si>
+  <si>
+    <t>Tipo di evento, determinato da un elenco</t>
+  </si>
+  <si>
+    <t>Nome del file originale</t>
+  </si>
+  <si>
+    <t>Dimensione del file in Mb</t>
+  </si>
+  <si>
+    <t>Testo in inglese</t>
+  </si>
+  <si>
+    <t>Link al luogo sul sito web geonames</t>
+  </si>
+  <si>
+    <t>Numero di ospiti all'evento</t>
+  </si>
+  <si>
+    <t>Identificatore univoco</t>
+  </si>
+  <si>
+    <t>Parole chiave associate alla scheda</t>
+  </si>
+  <si>
+    <t>Licenza d'uso del file multimediale</t>
+  </si>
+  <si>
+    <t>Citazione, come riportata nella storia originale</t>
+  </si>
+  <si>
+    <t>Importanza del personaggio nella storia</t>
+  </si>
+  <si>
+    <t>Numero di sequenza utilizzato per oggetti composti</t>
+  </si>
+  <si>
+    <t>Data e ora</t>
+  </si>
+  <si>
+    <t>URL che rimanda a una pagina esterna con ulteriori informazioni</t>
+  </si>
+  <si>
+    <t>L'evento è pericoloso?</t>
+  </si>
+  <si>
+    <t>Appartiene al seguente libro</t>
+  </si>
+  <si>
+    <t>link interno all'audio</t>
+  </si>
+  <si>
+    <t>link interno ai capitoli del libro</t>
+  </si>
+  <si>
+    <t>link interno all'edizione/alle edizioni</t>
+  </si>
+  <si>
+    <t>link interno a Personaggio/i</t>
+  </si>
+  <si>
+    <t>link interno a Antagonista/i</t>
+  </si>
+  <si>
+    <t>link interno a Protagonista/i</t>
+  </si>
+  <si>
+    <t>link interno a Evento/i</t>
+  </si>
+  <si>
+    <t>link interno a Immagine/i</t>
+  </si>
+  <si>
+    <t>link interno a Luogo/i</t>
+  </si>
+  <si>
+    <t>link interno a Video/i</t>
+  </si>
+  <si>
+    <t>link interno a Copertina/e del libro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1044,15 +1369,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,9 +1596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q916"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1282,12 +1608,12 @@
     <col min="3" max="3" width="24.33203125" customWidth="1"/>
     <col min="4" max="4" width="32.1640625" customWidth="1"/>
     <col min="5" max="5" width="32.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5" customWidth="1"/>
-    <col min="7" max="7" width="17.1640625" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="10" width="32.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="8.5" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="38.83203125" customWidth="1"/>
+    <col min="8" max="8" width="77.83203125" customWidth="1"/>
+    <col min="9" max="9" width="62.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" customWidth="1"/>
+    <col min="11" max="11" width="12.33203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="63" customWidth="1"/>
     <col min="13" max="13" width="29.1640625" customWidth="1"/>
     <col min="14" max="14" width="11.5" customWidth="1"/>
@@ -1346,16 +1672,16 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>259</v>
+        <v>231</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>260</v>
+        <v>232</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>261</v>
+        <v>233</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>262</v>
+        <v>234</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1363,9 +1689,15 @@
       <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
+      <c r="H2" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>338</v>
+      </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
       </c>
@@ -1395,6 +1727,15 @@
       <c r="G3" t="s">
         <v>25</v>
       </c>
+      <c r="H3" t="s">
+        <v>307</v>
+      </c>
+      <c r="I3" t="s">
+        <v>251</v>
+      </c>
+      <c r="J3" t="s">
+        <v>339</v>
+      </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
       </c>
@@ -1423,6 +1764,15 @@
       </c>
       <c r="G4" s="4" t="s">
         <v>33</v>
+      </c>
+      <c r="H4" t="s">
+        <v>308</v>
+      </c>
+      <c r="I4" t="s">
+        <v>252</v>
+      </c>
+      <c r="J4" t="s">
+        <v>32</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>34</v>
@@ -1453,6 +1803,15 @@
       </c>
       <c r="G5" s="4" t="s">
         <v>37</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>41</v>
@@ -1485,6 +1844,15 @@
       <c r="G6" s="4" t="s">
         <v>48</v>
       </c>
+      <c r="H6" t="s">
+        <v>309</v>
+      </c>
+      <c r="I6" t="s">
+        <v>253</v>
+      </c>
+      <c r="J6" t="s">
+        <v>340</v>
+      </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
       </c>
@@ -1516,6 +1884,15 @@
       <c r="G7" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="H7" t="s">
+        <v>310</v>
+      </c>
+      <c r="I7" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" t="s">
+        <v>54</v>
+      </c>
       <c r="L7" s="4" t="s">
         <v>56</v>
       </c>
@@ -1546,8 +1923,15 @@
       <c r="G8" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
+      <c r="H8" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="L8" s="4" t="s">
         <v>63</v>
       </c>
@@ -1579,8 +1963,15 @@
       <c r="G9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="H9" t="s">
+        <v>311</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>341</v>
+      </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
       </c>
@@ -1612,7 +2003,15 @@
       <c r="G10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="4"/>
+      <c r="H10" t="s">
+        <v>312</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="J10" t="s">
+        <v>342</v>
+      </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
       </c>
@@ -1645,8 +2044,15 @@
       <c r="G11" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="H11" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="J11" t="s">
+        <v>343</v>
+      </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
       </c>
@@ -1677,6 +2083,15 @@
       <c r="G12" t="s">
         <v>92</v>
       </c>
+      <c r="H12" t="s">
+        <v>314</v>
+      </c>
+      <c r="I12" t="s">
+        <v>258</v>
+      </c>
+      <c r="J12" t="s">
+        <v>344</v>
+      </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
       </c>
@@ -1706,6 +2121,15 @@
       <c r="G13" t="s">
         <v>100</v>
       </c>
+      <c r="H13" t="s">
+        <v>315</v>
+      </c>
+      <c r="I13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J13" t="s">
+        <v>345</v>
+      </c>
       <c r="L13" s="4" t="s">
         <v>101</v>
       </c>
@@ -1735,7 +2159,15 @@
       <c r="G14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I14" s="4"/>
+      <c r="H14" t="s">
+        <v>316</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J14" t="s">
+        <v>346</v>
+      </c>
       <c r="L14" s="4" t="s">
         <v>105</v>
       </c>
@@ -1767,6 +2199,15 @@
       <c r="G15" s="6" t="s">
         <v>113</v>
       </c>
+      <c r="H15" t="s">
+        <v>317</v>
+      </c>
+      <c r="I15" t="s">
+        <v>260</v>
+      </c>
+      <c r="J15" t="s">
+        <v>347</v>
+      </c>
       <c r="L15" s="4" t="s">
         <v>114</v>
       </c>
@@ -1795,6 +2236,15 @@
       </c>
       <c r="G16" s="4" t="s">
         <v>117</v>
+      </c>
+      <c r="H16" t="s">
+        <v>318</v>
+      </c>
+      <c r="I16" t="s">
+        <v>261</v>
+      </c>
+      <c r="J16" t="s">
+        <v>348</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>118</v>
@@ -1827,6 +2277,15 @@
       <c r="G17" t="s">
         <v>124</v>
       </c>
+      <c r="H17" t="s">
+        <v>319</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="J17" t="s">
+        <v>349</v>
+      </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
       </c>
@@ -1858,6 +2317,15 @@
       </c>
       <c r="G18" s="4" t="s">
         <v>132</v>
+      </c>
+      <c r="H18" t="s">
+        <v>320</v>
+      </c>
+      <c r="I18" t="s">
+        <v>262</v>
+      </c>
+      <c r="J18" t="s">
+        <v>350</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>133</v>
@@ -1893,7 +2361,15 @@
       <c r="G19" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="I19" s="4"/>
+      <c r="H19" t="s">
+        <v>136</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="J19" t="s">
+        <v>138</v>
+      </c>
       <c r="L19" s="4" t="s">
         <v>86</v>
       </c>
@@ -1924,6 +2400,15 @@
       <c r="G20" s="4" t="s">
         <v>144</v>
       </c>
+      <c r="H20" t="s">
+        <v>321</v>
+      </c>
+      <c r="I20" t="s">
+        <v>263</v>
+      </c>
+      <c r="J20" t="s">
+        <v>351</v>
+      </c>
       <c r="L20" s="4" t="s">
         <v>145</v>
       </c>
@@ -1951,7 +2436,18 @@
       <c r="E21" t="s">
         <v>150</v>
       </c>
-      <c r="G21" s="4"/>
+      <c r="G21" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="H21" t="s">
+        <v>322</v>
+      </c>
+      <c r="I21" t="s">
+        <v>264</v>
+      </c>
+      <c r="J21" t="s">
+        <v>352</v>
+      </c>
       <c r="L21" s="4" t="s">
         <v>151</v>
       </c>
@@ -1983,8 +2479,18 @@
       <c r="E22" t="s">
         <v>154</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="4"/>
+      <c r="G22" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="H22" t="s">
+        <v>323</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="J22" t="s">
+        <v>353</v>
+      </c>
       <c r="L22" s="4" t="s">
         <v>155</v>
       </c>
@@ -2013,7 +2519,18 @@
       <c r="E23" t="s">
         <v>160</v>
       </c>
-      <c r="G23" s="4"/>
+      <c r="G23" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H23" t="s">
+        <v>158</v>
+      </c>
+      <c r="I23" t="s">
+        <v>159</v>
+      </c>
+      <c r="J23" t="s">
+        <v>354</v>
+      </c>
       <c r="L23" s="4" t="s">
         <v>161</v>
       </c>
@@ -2042,7 +2559,18 @@
       <c r="E24" t="s">
         <v>168</v>
       </c>
-      <c r="G24" s="4"/>
+      <c r="G24" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="H24" t="s">
+        <v>324</v>
+      </c>
+      <c r="I24" t="s">
+        <v>266</v>
+      </c>
+      <c r="J24" t="s">
+        <v>355</v>
+      </c>
       <c r="L24" s="4" t="s">
         <v>169</v>
       </c>
@@ -2069,7 +2597,18 @@
       <c r="E25" t="s">
         <v>175</v>
       </c>
-      <c r="G25" s="4"/>
+      <c r="G25" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H25" t="s">
+        <v>325</v>
+      </c>
+      <c r="I25" t="s">
+        <v>267</v>
+      </c>
+      <c r="J25" t="s">
+        <v>356</v>
+      </c>
       <c r="L25" s="4" t="s">
         <v>176</v>
       </c>
@@ -2096,8 +2635,18 @@
       <c r="E26" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="G26" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="H26" t="s">
+        <v>326</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="J26" t="s">
+        <v>357</v>
+      </c>
       <c r="L26" s="4" t="s">
         <v>184</v>
       </c>
@@ -2114,35 +2663,35 @@
       <c r="A27" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="H27" t="s">
+        <v>327</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="J27" t="s">
+        <v>358</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C27" t="s">
+      <c r="M27" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="D27" t="s">
-        <v>190</v>
-      </c>
-      <c r="E27" t="s">
-        <v>191</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="H27" t="s">
-        <v>189</v>
-      </c>
-      <c r="I27" t="s">
-        <v>190</v>
-      </c>
-      <c r="J27" t="s">
-        <v>191</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>193</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>186</v>
@@ -2152,37 +2701,37 @@
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C28" t="s">
+        <v>192</v>
+      </c>
+      <c r="D28" t="s">
+        <v>193</v>
+      </c>
+      <c r="E28" t="s">
         <v>194</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="G28" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H28" t="s">
+        <v>328</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="J28" t="s">
+        <v>359</v>
+      </c>
+      <c r="L28" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C28" t="s">
+      <c r="M28" s="4" t="s">
         <v>196</v>
-      </c>
-      <c r="D28" t="s">
-        <v>197</v>
-      </c>
-      <c r="E28" t="s">
-        <v>198</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="H28" t="s">
-        <v>196</v>
-      </c>
-      <c r="I28" t="s">
-        <v>197</v>
-      </c>
-      <c r="J28" t="s">
-        <v>198</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="M28" s="4" t="s">
-        <v>200</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>186</v>
@@ -2190,27 +2739,37 @@
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="G29" s="4"/>
-      <c r="I29" s="4"/>
+        <v>197</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="H29" t="s">
+        <v>329</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="J29" t="s">
+        <v>360</v>
+      </c>
       <c r="L29" s="4" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>186</v>
@@ -2218,29 +2777,37 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
+        <v>200</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="G30" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>361</v>
+      </c>
       <c r="L30" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>186</v>
@@ -2250,26 +2817,37 @@
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C31" t="s">
-        <v>217</v>
-      </c>
-      <c r="D31" t="s">
-        <v>218</v>
+        <v>205</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>206</v>
       </c>
       <c r="E31" t="s">
-        <v>219</v>
-      </c>
-      <c r="G31" s="4"/>
+        <v>207</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H31" t="s">
+        <v>331</v>
+      </c>
+      <c r="I31" t="s">
+        <v>271</v>
+      </c>
+      <c r="J31" t="s">
+        <v>362</v>
+      </c>
       <c r="L31" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>186</v>
@@ -2277,26 +2855,37 @@
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="C32" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="D32" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="E32" t="s">
-        <v>224</v>
-      </c>
-      <c r="G32" s="4"/>
+        <v>212</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="H32" t="s">
+        <v>332</v>
+      </c>
+      <c r="I32" t="s">
+        <v>272</v>
+      </c>
+      <c r="J32" t="s">
+        <v>363</v>
+      </c>
       <c r="L32" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>186</v>
@@ -2304,25 +2893,37 @@
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>229</v>
+        <v>213</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="G33" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="H33" t="s">
+        <v>333</v>
+      </c>
+      <c r="I33" t="s">
+        <v>273</v>
+      </c>
+      <c r="J33" t="s">
+        <v>364</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>230</v>
+        <v>214</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>231</v>
+        <v>215</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>186</v>
@@ -2330,29 +2931,37 @@
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
+        <v>216</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>365</v>
+      </c>
       <c r="L34" s="4" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>186</v>
@@ -2360,26 +2969,37 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>240</v>
+        <v>219</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>220</v>
       </c>
       <c r="C35" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="D35" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="E35" t="s">
-        <v>243</v>
-      </c>
-      <c r="G35" s="4"/>
+        <v>223</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H35" t="s">
+        <v>335</v>
+      </c>
+      <c r="I35" t="s">
+        <v>275</v>
+      </c>
+      <c r="J35" t="s">
+        <v>366</v>
+      </c>
       <c r="L35" s="4" t="s">
-        <v>244</v>
+        <v>224</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>245</v>
+        <v>225</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>186</v>
@@ -2388,27 +3008,37 @@
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="G36" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>247</v>
-      </c>
-      <c r="C36" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="E36" t="s">
-        <v>250</v>
-      </c>
-      <c r="G36" s="4"/>
-      <c r="I36" s="4"/>
+      <c r="H36" t="s">
+        <v>336</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="J36" t="s">
+        <v>367</v>
+      </c>
       <c r="L36" s="4" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>186</v>
@@ -2418,25 +3048,37 @@
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>257</v>
+        <v>229</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="H37" t="s">
+        <v>337</v>
+      </c>
+      <c r="I37" t="s">
+        <v>277</v>
+      </c>
+      <c r="J37" t="s">
+        <v>368</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>258</v>
+        <v>230</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>186</v>

</xml_diff>

<commit_message>
Adaptations Data Model for Legal info on Resources
Update deprecated functions
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE474518-9F78-CE44-95D9-10D721C974DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267FB03F-9149-104C-8369-9BC49C0E0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$37</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="384">
   <si>
     <t>name</t>
   </si>
@@ -877,9 +877,6 @@
     <t>Urheber:in</t>
   </si>
   <si>
-    <t>Auteur·ice</t>
-  </si>
-  <si>
     <t>Importance of the character in the story</t>
   </si>
   <si>
@@ -1280,18 +1277,80 @@
   </si>
   <si>
     <t>link interno a Copertina/e del libro</t>
+  </si>
+  <si>
+    <t>hasAuthorshipResource</t>
+  </si>
+  <si>
+    <t>Author of the resource</t>
+  </si>
+  <si>
+    <t>Autor der Resource</t>
+  </si>
+  <si>
+    <t>Auteur·rice</t>
+  </si>
+  <si>
+    <t>Auteur·rice de la ressource</t>
+  </si>
+  <si>
+    <t>Autore della risorsa</t>
+  </si>
+  <si>
+    <t>hasCopyrightResource</t>
+  </si>
+  <si>
+    <t>hasLicenseResource</t>
+  </si>
+  <si>
+    <t>Copyright of the resource</t>
+  </si>
+  <si>
+    <t>License of the resource</t>
+  </si>
+  <si>
+    <t>Lizenz der Resource</t>
+  </si>
+  <si>
+    <t>Urheberrecht der Resource</t>
+  </si>
+  <si>
+    <t>Licence de la ressource</t>
+  </si>
+  <si>
+    <t>Droits d'auteur de la ressource</t>
+  </si>
+  <si>
+    <t>Copyright della risorsa</t>
+  </si>
+  <si>
+    <t>Licenza della risorsa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1342,6 +1401,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1369,15 +1435,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1596,9 +1665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q916"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1680,8 +1749,8 @@
       <c r="C2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>234</v>
+      <c r="D2" s="9" t="s">
+        <v>371</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1690,13 +1759,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
@@ -1728,13 +1797,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
@@ -1766,10 +1835,10 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1845,13 +1914,13 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -1885,7 +1954,7 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -1927,7 +1996,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>62</v>
@@ -1964,13 +2033,13 @@
         <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
@@ -2004,13 +2073,13 @@
         <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
@@ -2045,13 +2114,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
@@ -2084,13 +2153,13 @@
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
@@ -2122,13 +2191,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>101</v>
@@ -2160,13 +2229,13 @@
         <v>104</v>
       </c>
       <c r="H14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>105</v>
@@ -2200,13 +2269,13 @@
         <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>114</v>
@@ -2238,13 +2307,13 @@
         <v>117</v>
       </c>
       <c r="H16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>118</v>
@@ -2278,13 +2347,13 @@
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
@@ -2319,13 +2388,13 @@
         <v>132</v>
       </c>
       <c r="H18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>133</v>
@@ -2401,13 +2470,13 @@
         <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>145</v>
@@ -2437,16 +2506,16 @@
         <v>150</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>151</v>
@@ -2480,16 +2549,16 @@
         <v>154</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>155</v>
@@ -2520,7 +2589,7 @@
         <v>160</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H23" t="s">
         <v>158</v>
@@ -2529,7 +2598,7 @@
         <v>159</v>
       </c>
       <c r="J23" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>161</v>
@@ -2560,16 +2629,16 @@
         <v>168</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>169</v>
@@ -2598,16 +2667,16 @@
         <v>175</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>176</v>
@@ -2636,16 +2705,16 @@
         <v>183</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>184</v>
@@ -2664,28 +2733,28 @@
         <v>187</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>188</v>
@@ -2716,16 +2785,16 @@
         <v>194</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>195</v>
@@ -2742,28 +2811,28 @@
         <v>197</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>198</v>
@@ -2780,28 +2849,28 @@
         <v>200</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>201</v>
@@ -2832,16 +2901,16 @@
         <v>207</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>201</v>
@@ -2870,16 +2939,16 @@
         <v>212</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>201</v>
@@ -2896,28 +2965,28 @@
         <v>213</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J33" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>214</v>
@@ -2934,28 +3003,28 @@
         <v>216</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>295</v>
-      </c>
       <c r="E34" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>217</v>
@@ -2984,16 +3053,16 @@
         <v>223</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I35" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J35" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>224</v>
@@ -3011,28 +3080,28 @@
         <v>226</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>227</v>
@@ -3051,28 +3120,28 @@
         <v>229</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J37" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>217</v>
@@ -3084,9 +3153,123 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update functions and Data Model (#50)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE474518-9F78-CE44-95D9-10D721C974DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267FB03F-9149-104C-8369-9BC49C0E0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$37</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="384">
   <si>
     <t>name</t>
   </si>
@@ -877,9 +877,6 @@
     <t>Urheber:in</t>
   </si>
   <si>
-    <t>Auteur·ice</t>
-  </si>
-  <si>
     <t>Importance of the character in the story</t>
   </si>
   <si>
@@ -1280,18 +1277,80 @@
   </si>
   <si>
     <t>link interno a Copertina/e del libro</t>
+  </si>
+  <si>
+    <t>hasAuthorshipResource</t>
+  </si>
+  <si>
+    <t>Author of the resource</t>
+  </si>
+  <si>
+    <t>Autor der Resource</t>
+  </si>
+  <si>
+    <t>Auteur·rice</t>
+  </si>
+  <si>
+    <t>Auteur·rice de la ressource</t>
+  </si>
+  <si>
+    <t>Autore della risorsa</t>
+  </si>
+  <si>
+    <t>hasCopyrightResource</t>
+  </si>
+  <si>
+    <t>hasLicenseResource</t>
+  </si>
+  <si>
+    <t>Copyright of the resource</t>
+  </si>
+  <si>
+    <t>License of the resource</t>
+  </si>
+  <si>
+    <t>Lizenz der Resource</t>
+  </si>
+  <si>
+    <t>Urheberrecht der Resource</t>
+  </si>
+  <si>
+    <t>Licence de la ressource</t>
+  </si>
+  <si>
+    <t>Droits d'auteur de la ressource</t>
+  </si>
+  <si>
+    <t>Copyright della risorsa</t>
+  </si>
+  <si>
+    <t>Licenza della risorsa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1342,6 +1401,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1369,15 +1435,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1596,9 +1665,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q916"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J40" sqref="J40"/>
+      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1680,8 +1749,8 @@
       <c r="C2" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>234</v>
+      <c r="D2" s="9" t="s">
+        <v>371</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1690,13 +1759,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
@@ -1728,13 +1797,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="I3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
@@ -1766,10 +1835,10 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1845,13 +1914,13 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="I6" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J6" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -1885,7 +1954,7 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -1927,7 +1996,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>62</v>
@@ -1964,13 +2033,13 @@
         <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
@@ -2004,13 +2073,13 @@
         <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
@@ -2045,13 +2114,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="J11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
@@ -2084,13 +2153,13 @@
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="I12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J12" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
@@ -2122,13 +2191,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="J13" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>101</v>
@@ -2160,13 +2229,13 @@
         <v>104</v>
       </c>
       <c r="H14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>105</v>
@@ -2200,13 +2269,13 @@
         <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>114</v>
@@ -2238,13 +2307,13 @@
         <v>117</v>
       </c>
       <c r="H16" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I16" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J16" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>118</v>
@@ -2278,13 +2347,13 @@
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J17" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
@@ -2319,13 +2388,13 @@
         <v>132</v>
       </c>
       <c r="H18" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>133</v>
@@ -2401,13 +2470,13 @@
         <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="J20" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>145</v>
@@ -2437,16 +2506,16 @@
         <v>150</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="H21" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="I21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="J21" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>151</v>
@@ -2480,16 +2549,16 @@
         <v>154</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H22" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="J22" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>155</v>
@@ -2520,7 +2589,7 @@
         <v>160</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="H23" t="s">
         <v>158</v>
@@ -2529,7 +2598,7 @@
         <v>159</v>
       </c>
       <c r="J23" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>161</v>
@@ -2560,16 +2629,16 @@
         <v>168</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I24" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J24" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>169</v>
@@ -2598,16 +2667,16 @@
         <v>175</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="H25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="J25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>176</v>
@@ -2636,16 +2705,16 @@
         <v>183</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H26" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="L26" s="4" t="s">
         <v>184</v>
@@ -2664,28 +2733,28 @@
         <v>187</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H27" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J27" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L27" s="4" t="s">
         <v>188</v>
@@ -2716,16 +2785,16 @@
         <v>194</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H28" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J28" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L28" s="4" t="s">
         <v>195</v>
@@ -2742,28 +2811,28 @@
         <v>197</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H29" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="J29" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>198</v>
@@ -2780,28 +2849,28 @@
         <v>200</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="J30" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="L30" s="4" t="s">
         <v>201</v>
@@ -2832,16 +2901,16 @@
         <v>207</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H31" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I31" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J31" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>201</v>
@@ -2870,16 +2939,16 @@
         <v>212</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H32" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>201</v>
@@ -2896,28 +2965,28 @@
         <v>213</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H33" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I33" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J33" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>214</v>
@@ -2934,28 +3003,28 @@
         <v>216</v>
       </c>
       <c r="B34" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="C34" s="8" t="s">
-        <v>289</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>295</v>
-      </c>
       <c r="E34" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>217</v>
@@ -2984,16 +3053,16 @@
         <v>223</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="I35" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J35" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L35" s="4" t="s">
         <v>224</v>
@@ -3011,28 +3080,28 @@
         <v>226</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H36" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>227</v>
@@ -3051,28 +3120,28 @@
         <v>229</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H37" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I37" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J37" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="L37" s="4" t="s">
         <v>217</v>
@@ -3084,9 +3153,123 @@
         <v>186</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>369</v>
+      </c>
+      <c r="H38" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>373</v>
+      </c>
+      <c r="L38" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M38" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N38" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="L39" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
+        <v>375</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>377</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>378</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>380</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
ontology add permissions to properties and resources
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267FB03F-9149-104C-8369-9BC49C0E0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DD0CF34-CFFF-B040-B682-07C0B2191551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="386">
   <si>
     <t>name</t>
   </si>
@@ -1325,18 +1325,31 @@
   </si>
   <si>
     <t>Licenza della risorsa</t>
+  </si>
+  <si>
+    <t>default_permissions_overrule</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1408,6 +1421,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.199999999999999"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1435,18 +1455,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1665,9 +1687,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q916"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
+      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1683,8 +1705,8 @@
     <col min="9" max="9" width="62.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="44.1640625" customWidth="1"/>
     <col min="11" max="11" width="12.33203125" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="63" customWidth="1"/>
-    <col min="13" max="13" width="29.1640625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
     <col min="14" max="14" width="11.5" customWidth="1"/>
     <col min="15" max="15" width="22.83203125" customWidth="1"/>
     <col min="16" max="16" width="21.6640625" customWidth="1"/>
@@ -1738,6 +1760,9 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="12" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2050,7 +2075,9 @@
       <c r="N9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="4"/>
+      <c r="P9" s="13" t="s">
+        <v>385</v>
+      </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ontology add permissions to properties and resources (#52)
Co-authored-by: Johannes Nussbaum <johannes.nussbaum@dasch.swiss>
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{267FB03F-9149-104C-8369-9BC49C0E0A7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B570E6D-D602-424D-A394-2B9295B0780B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="386">
   <si>
     <t>name</t>
   </si>
@@ -1325,18 +1325,31 @@
   </si>
   <si>
     <t>Licenza della risorsa</t>
+  </si>
+  <si>
+    <t>default_permissions_overrule</t>
+  </si>
+  <si>
+    <t>private</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1408,6 +1421,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10.199999999999999"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1435,18 +1455,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1667,7 +1689,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L40" sqref="L40"/>
+      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1738,6 +1760,9 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="12" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -2050,7 +2075,9 @@
       <c r="N9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="4"/>
+      <c r="P9" s="13" t="s">
+        <v>385</v>
+      </c>
       <c r="Q9" s="4"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
addition of isPartOfCharacter Property
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B570E6D-D602-424D-A394-2B9295B0780B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72DA4A2-C37E-6243-9CCF-7D161080444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$38</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
   <si>
     <t>name</t>
   </si>
@@ -1331,18 +1331,40 @@
   </si>
   <si>
     <t>private</t>
+  </si>
+  <si>
+    <t>isPartOfCharacter</t>
+  </si>
+  <si>
+    <t>Character(s) on the image</t>
+  </si>
+  <si>
+    <t>Personnage(s) sur l'image</t>
+  </si>
+  <si>
+    <t>Personaggio/i nell'immagine</t>
+  </si>
+  <si>
+    <t>Charakter(e) auf dem Bild</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1455,20 +1477,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1685,11 +1709,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q916"/>
+  <dimension ref="A1:Q917"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P12" sqref="P12"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2756,38 +2780,38 @@
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>302</v>
-      </c>
-      <c r="H27" t="s">
-        <v>326</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="J27" t="s">
-        <v>357</v>
+      <c r="A27" s="14" t="s">
+        <v>386</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="C27" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="G27" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="H27" s="15" t="s">
+        <v>390</v>
+      </c>
+      <c r="I27" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>389</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="M27" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
+      </c>
+      <c r="M27" s="15" t="s">
+        <v>202</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>186</v>
@@ -2797,75 +2821,77 @@
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C28" t="s">
-        <v>192</v>
-      </c>
-      <c r="D28" t="s">
-        <v>193</v>
-      </c>
-      <c r="E28" t="s">
-        <v>194</v>
+        <v>187</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>284</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="H28" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J28" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>186</v>
       </c>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>280</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>297</v>
+        <v>190</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C29" t="s">
+        <v>192</v>
+      </c>
+      <c r="D29" t="s">
+        <v>193</v>
+      </c>
+      <c r="E29" t="s">
+        <v>194</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>240</v>
+        <v>279</v>
       </c>
       <c r="H29" t="s">
-        <v>328</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>268</v>
+        <v>327</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>303</v>
       </c>
       <c r="J29" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>186</v>
@@ -2873,71 +2899,69 @@
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>329</v>
+        <v>240</v>
+      </c>
+      <c r="H30" t="s">
+        <v>328</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>360</v>
+        <v>268</v>
+      </c>
+      <c r="J30" t="s">
+        <v>359</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="P30" s="4"/>
-      <c r="Q30" s="4"/>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>204</v>
-      </c>
-      <c r="C31" t="s">
-        <v>205</v>
+        <v>200</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>286</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="E31" t="s">
-        <v>207</v>
+        <v>290</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>247</v>
-      </c>
-      <c r="H31" t="s">
-        <v>330</v>
-      </c>
-      <c r="I31" t="s">
-        <v>270</v>
-      </c>
-      <c r="J31" t="s">
-        <v>361</v>
+        <v>241</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>360</v>
       </c>
       <c r="L31" s="4" t="s">
         <v>201</v>
@@ -2948,34 +2972,36 @@
       <c r="N31" s="4" t="s">
         <v>186</v>
       </c>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="C32" t="s">
-        <v>210</v>
-      </c>
-      <c r="D32" t="s">
-        <v>211</v>
+        <v>205</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>206</v>
       </c>
       <c r="E32" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="J32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="L32" s="4" t="s">
         <v>201</v>
@@ -2989,37 +3015,37 @@
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>291</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>298</v>
+        <v>208</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="C33" t="s">
+        <v>210</v>
+      </c>
+      <c r="D33" t="s">
+        <v>211</v>
+      </c>
+      <c r="E33" t="s">
+        <v>212</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="H33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I33" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="J33" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>186</v>
@@ -3027,37 +3053,37 @@
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>333</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>364</v>
+        <v>242</v>
+      </c>
+      <c r="H34" t="s">
+        <v>332</v>
+      </c>
+      <c r="I34" t="s">
+        <v>272</v>
+      </c>
+      <c r="J34" t="s">
+        <v>363</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>186</v>
@@ -3065,189 +3091,189 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C35" t="s">
-        <v>221</v>
-      </c>
-      <c r="D35" t="s">
-        <v>222</v>
-      </c>
-      <c r="E35" t="s">
-        <v>223</v>
+        <v>293</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>299</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="H35" t="s">
-        <v>334</v>
-      </c>
-      <c r="I35" t="s">
-        <v>274</v>
-      </c>
-      <c r="J35" t="s">
-        <v>365</v>
+        <v>243</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>364</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="P35" s="4"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>282</v>
+        <v>220</v>
+      </c>
+      <c r="C36" t="s">
+        <v>221</v>
+      </c>
+      <c r="D36" t="s">
+        <v>222</v>
+      </c>
+      <c r="E36" t="s">
+        <v>223</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H36" t="s">
-        <v>335</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>275</v>
+        <v>334</v>
+      </c>
+      <c r="I36" t="s">
+        <v>274</v>
       </c>
       <c r="J36" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>186</v>
       </c>
       <c r="P36" s="4"/>
-      <c r="Q36" s="4"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H37" t="s">
-        <v>336</v>
-      </c>
-      <c r="I37" t="s">
-        <v>276</v>
+        <v>335</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>275</v>
       </c>
       <c r="J37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>217</v>
+        <v>227</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>186</v>
       </c>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="E38" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="G38" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>370</v>
-      </c>
-      <c r="I38" s="9" t="s">
-        <v>372</v>
-      </c>
-      <c r="J38" s="11" t="s">
-        <v>373</v>
+      <c r="A38" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" t="s">
+        <v>336</v>
+      </c>
+      <c r="I38" t="s">
+        <v>276</v>
+      </c>
+      <c r="J38" t="s">
+        <v>367</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>18</v>
+        <v>230</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>19</v>
+        <v>186</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="10" t="s">
-        <v>374</v>
+      <c r="A39" s="9" t="s">
+        <v>368</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="C39" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>381</v>
+        <v>369</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>372</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>376</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>379</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>381</v>
+        <v>369</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>372</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>382</v>
+        <v>373</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="M39" s="4" t="s">
         <v>18</v>
@@ -3258,46 +3284,83 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>376</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>379</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>381</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>382</v>
+      </c>
+      <c r="L40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="10" t="s">
         <v>375</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B41" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C41" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="E40" s="11" t="s">
+      <c r="E41" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>377</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="H41" s="11" t="s">
         <v>378</v>
       </c>
-      <c r="I40" s="11" t="s">
+      <c r="I41" s="11" t="s">
         <v>380</v>
       </c>
-      <c r="J40" s="11" t="s">
+      <c r="J41" s="11" t="s">
         <v>383</v>
       </c>
-      <c r="L40" s="4" t="s">
+      <c r="L41" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="M40" s="4" t="s">
+      <c r="M41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="N40" s="4" t="s">
+      <c r="N41" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="O40" s="4" t="s">
+      <c r="O41" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4173,8 +4236,9 @@
     <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:Q37" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="property-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="property-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
scripts changes for metadata
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72DA4A2-C37E-6243-9CCF-7D161080444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3195EAA-FB5A-F642-BCE2-53D0DB4EFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="392">
   <si>
     <t>name</t>
   </si>
@@ -1346,18 +1346,28 @@
   </si>
   <si>
     <t>Charakter(e) auf dem Bild</t>
+  </si>
+  <si>
+    <t>Textarea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1477,22 +1487,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1713,7 +1724,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1860,8 +1871,8 @@
       <c r="M3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>27</v>
+      <c r="N3" s="16" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
scripts changes for metadata (#61)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72DA4A2-C37E-6243-9CCF-7D161080444B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3195EAA-FB5A-F642-BCE2-53D0DB4EFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7060" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3800" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="392">
   <si>
     <t>name</t>
   </si>
@@ -1346,18 +1346,28 @@
   </si>
   <si>
     <t>Charakter(e) auf dem Bild</t>
+  </si>
+  <si>
+    <t>Textarea</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1477,22 +1487,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1713,7 +1724,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
+      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1860,8 +1871,8 @@
       <c r="M3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="4" t="s">
-        <v>27</v>
+      <c r="N3" s="16" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
change isPartOfBook to isPartOfBookChapter
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3195EAA-FB5A-F642-BCE2-53D0DB4EFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01245E07-5910-8340-8954-DB4E1658C0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
   <si>
     <t>name</t>
   </si>
@@ -712,27 +712,9 @@
     <t>Checkbox</t>
   </si>
   <si>
-    <t>isPartOfBook</t>
-  </si>
-  <si>
-    <t>Part of Book</t>
-  </si>
-  <si>
-    <t>Teil des Buches</t>
-  </si>
-  <si>
-    <t>Appartient au Livre</t>
-  </si>
-  <si>
-    <t>Appartiene al libro</t>
-  </si>
-  <si>
     <t>isPartOf, schema:isPartOf, crm:P5i_forms_part_of</t>
   </si>
   <si>
-    <t>:Book</t>
-  </si>
-  <si>
     <t>Searchbox</t>
   </si>
   <si>
@@ -892,9 +874,6 @@
     <t>Is the event dangerous?</t>
   </si>
   <si>
-    <t>Belongs to following book</t>
-  </si>
-  <si>
     <t>internal link to the Edition(s)</t>
   </si>
   <si>
@@ -976,9 +955,6 @@
     <t>L'événement est-il dangereux ?</t>
   </si>
   <si>
-    <t>Appartient au livre suivant</t>
-  </si>
-  <si>
     <t>lien interne vers l'(les) édition(s)</t>
   </si>
   <si>
@@ -1150,9 +1126,6 @@
     <t>Ist das Ereignis gefährlich?</t>
   </si>
   <si>
-    <t>Gehört zu folgendem Buch</t>
-  </si>
-  <si>
     <t>Interner Link zu Audio</t>
   </si>
   <si>
@@ -1243,9 +1216,6 @@
     <t>L'evento è pericoloso?</t>
   </si>
   <si>
-    <t>Appartiene al seguente libro</t>
-  </si>
-  <si>
     <t>link interno all'audio</t>
   </si>
   <si>
@@ -1349,18 +1319,52 @@
   </si>
   <si>
     <t>Textarea</t>
+  </si>
+  <si>
+    <t>isPartOfBookChapter</t>
+  </si>
+  <si>
+    <t>Appartient au chapitre</t>
+  </si>
+  <si>
+    <t>Teil des Kapitels</t>
+  </si>
+  <si>
+    <t>Part of chapter</t>
+  </si>
+  <si>
+    <t>Appartiene al capitolo</t>
+  </si>
+  <si>
+    <t>Belongs to following chapter</t>
+  </si>
+  <si>
+    <t>Gehört zu folgendem Kapitel</t>
+  </si>
+  <si>
+    <t>Appartient au chapitre suivant</t>
+  </si>
+  <si>
+    <t>Appartiene al seguente capitolo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1487,23 +1491,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1722,9 +1728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1796,21 +1802,21 @@
         <v>14</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1819,13 +1825,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
@@ -1857,13 +1863,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="I3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J3" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
@@ -1872,7 +1878,7 @@
         <v>18</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1895,10 +1901,10 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="I4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1974,13 +1980,13 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J6" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -2014,7 +2020,7 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -2056,7 +2062,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>62</v>
@@ -2093,13 +2099,13 @@
         <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
@@ -2111,7 +2117,7 @@
         <v>27</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
@@ -2135,13 +2141,13 @@
         <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J10" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
@@ -2176,13 +2182,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J11" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
@@ -2215,13 +2221,13 @@
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="I12" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="J12" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
@@ -2253,13 +2259,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I13" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J13" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>101</v>
@@ -2291,13 +2297,13 @@
         <v>104</v>
       </c>
       <c r="H14" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J14" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>105</v>
@@ -2331,13 +2337,13 @@
         <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="I15" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="J15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>114</v>
@@ -2369,13 +2375,13 @@
         <v>117</v>
       </c>
       <c r="H16" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="I16" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="J16" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>118</v>
@@ -2409,13 +2415,13 @@
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="J17" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
@@ -2450,13 +2456,13 @@
         <v>132</v>
       </c>
       <c r="H18" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="I18" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J18" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>133</v>
@@ -2532,13 +2538,13 @@
         <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I20" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="J20" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>145</v>
@@ -2568,16 +2574,16 @@
         <v>150</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H21" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="I21" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="J21" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>151</v>
@@ -2611,16 +2617,16 @@
         <v>154</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H22" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J22" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>155</v>
@@ -2651,7 +2657,7 @@
         <v>160</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H23" t="s">
         <v>158</v>
@@ -2660,7 +2666,7 @@
         <v>159</v>
       </c>
       <c r="J23" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>161</v>
@@ -2691,16 +2697,16 @@
         <v>168</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H24" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I24" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="J24" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>169</v>
@@ -2729,16 +2735,16 @@
         <v>175</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H25" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I25" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J25" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>176</v>
@@ -2751,537 +2757,537 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="M26" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="N26" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="H26" t="s">
-        <v>325</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="J26" t="s">
-        <v>356</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="H28" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="J28" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="H29" t="s">
+        <v>318</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="J29" t="s">
+        <v>348</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M29" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C29" t="s">
-        <v>192</v>
-      </c>
-      <c r="D29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" t="s">
-        <v>194</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="H29" t="s">
-        <v>327</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="J29" t="s">
-        <v>358</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="N29" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H30" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="J30" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E32" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H32" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I32" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="J32" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E33" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H33" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="I33" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="J33" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H34" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I34" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J34" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H36" t="s">
+        <v>325</v>
+      </c>
+      <c r="I36" t="s">
+        <v>266</v>
+      </c>
+      <c r="J36" t="s">
+        <v>355</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C36" t="s">
-        <v>221</v>
-      </c>
-      <c r="D36" t="s">
-        <v>222</v>
-      </c>
-      <c r="E36" t="s">
-        <v>223</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="H36" t="s">
-        <v>334</v>
-      </c>
-      <c r="I36" t="s">
-        <v>274</v>
-      </c>
-      <c r="J36" t="s">
-        <v>365</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="N36" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P36" s="4"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H37" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="J37" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H38" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="I38" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="J38" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>17</v>
@@ -3295,31 +3301,31 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>49</v>
@@ -3333,31 +3339,31 @@
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
change isPartOfBook to isPartOfBookChapter (#63)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10824"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3195EAA-FB5A-F642-BCE2-53D0DB4EFEB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01245E07-5910-8340-8954-DB4E1658C0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
   <si>
     <t>name</t>
   </si>
@@ -712,27 +712,9 @@
     <t>Checkbox</t>
   </si>
   <si>
-    <t>isPartOfBook</t>
-  </si>
-  <si>
-    <t>Part of Book</t>
-  </si>
-  <si>
-    <t>Teil des Buches</t>
-  </si>
-  <si>
-    <t>Appartient au Livre</t>
-  </si>
-  <si>
-    <t>Appartiene al libro</t>
-  </si>
-  <si>
     <t>isPartOf, schema:isPartOf, crm:P5i_forms_part_of</t>
   </si>
   <si>
-    <t>:Book</t>
-  </si>
-  <si>
     <t>Searchbox</t>
   </si>
   <si>
@@ -892,9 +874,6 @@
     <t>Is the event dangerous?</t>
   </si>
   <si>
-    <t>Belongs to following book</t>
-  </si>
-  <si>
     <t>internal link to the Edition(s)</t>
   </si>
   <si>
@@ -976,9 +955,6 @@
     <t>L'événement est-il dangereux ?</t>
   </si>
   <si>
-    <t>Appartient au livre suivant</t>
-  </si>
-  <si>
     <t>lien interne vers l'(les) édition(s)</t>
   </si>
   <si>
@@ -1150,9 +1126,6 @@
     <t>Ist das Ereignis gefährlich?</t>
   </si>
   <si>
-    <t>Gehört zu folgendem Buch</t>
-  </si>
-  <si>
     <t>Interner Link zu Audio</t>
   </si>
   <si>
@@ -1243,9 +1216,6 @@
     <t>L'evento è pericoloso?</t>
   </si>
   <si>
-    <t>Appartiene al seguente libro</t>
-  </si>
-  <si>
     <t>link interno all'audio</t>
   </si>
   <si>
@@ -1349,18 +1319,52 @@
   </si>
   <si>
     <t>Textarea</t>
+  </si>
+  <si>
+    <t>isPartOfBookChapter</t>
+  </si>
+  <si>
+    <t>Appartient au chapitre</t>
+  </si>
+  <si>
+    <t>Teil des Kapitels</t>
+  </si>
+  <si>
+    <t>Part of chapter</t>
+  </si>
+  <si>
+    <t>Appartiene al capitolo</t>
+  </si>
+  <si>
+    <t>Belongs to following chapter</t>
+  </si>
+  <si>
+    <t>Gehört zu folgendem Kapitel</t>
+  </si>
+  <si>
+    <t>Appartient au chapitre suivant</t>
+  </si>
+  <si>
+    <t>Appartiene al seguente capitolo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1487,23 +1491,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1722,9 +1728,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q917"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P15" sqref="P15"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1796,21 +1802,21 @@
         <v>14</v>
       </c>
       <c r="P1" s="12" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>371</v>
+        <v>361</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1819,13 +1825,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
@@ -1857,13 +1863,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="I3" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="J3" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
@@ -1872,7 +1878,7 @@
         <v>18</v>
       </c>
       <c r="N3" s="16" t="s">
-        <v>391</v>
+        <v>381</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1895,10 +1901,10 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="I4" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1974,13 +1980,13 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="I6" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J6" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -2014,7 +2020,7 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -2056,7 +2062,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>62</v>
@@ -2093,13 +2099,13 @@
         <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
@@ -2111,7 +2117,7 @@
         <v>27</v>
       </c>
       <c r="P9" s="13" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
@@ -2135,13 +2141,13 @@
         <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J10" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
@@ -2176,13 +2182,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="J11" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
@@ -2215,13 +2221,13 @@
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="I12" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="J12" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
@@ -2253,13 +2259,13 @@
         <v>100</v>
       </c>
       <c r="H13" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="I13" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J13" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="L13" s="4" t="s">
         <v>101</v>
@@ -2291,13 +2297,13 @@
         <v>104</v>
       </c>
       <c r="H14" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="J14" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>105</v>
@@ -2331,13 +2337,13 @@
         <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="I15" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="J15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="L15" s="4" t="s">
         <v>114</v>
@@ -2369,13 +2375,13 @@
         <v>117</v>
       </c>
       <c r="H16" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="I16" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="J16" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="L16" s="4" t="s">
         <v>118</v>
@@ -2409,13 +2415,13 @@
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>318</v>
+        <v>310</v>
       </c>
       <c r="I17" s="8" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="J17" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
@@ -2450,13 +2456,13 @@
         <v>132</v>
       </c>
       <c r="H18" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="I18" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="J18" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="L18" s="4" t="s">
         <v>133</v>
@@ -2532,13 +2538,13 @@
         <v>144</v>
       </c>
       <c r="H20" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="I20" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="J20" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="L20" s="4" t="s">
         <v>145</v>
@@ -2568,16 +2574,16 @@
         <v>150</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="H21" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="I21" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="J21" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>151</v>
@@ -2611,16 +2617,16 @@
         <v>154</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="H22" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J22" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="L22" s="4" t="s">
         <v>155</v>
@@ -2651,7 +2657,7 @@
         <v>160</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="H23" t="s">
         <v>158</v>
@@ -2660,7 +2666,7 @@
         <v>159</v>
       </c>
       <c r="J23" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="L23" s="4" t="s">
         <v>161</v>
@@ -2691,16 +2697,16 @@
         <v>168</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H24" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="I24" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="J24" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>169</v>
@@ -2729,16 +2735,16 @@
         <v>175</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H25" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="I25" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J25" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="L25" s="4" t="s">
         <v>176</v>
@@ -2751,537 +2757,537 @@
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+      <c r="A26" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>385</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>384</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>383</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>386</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>387</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>388</v>
+      </c>
+      <c r="I26" s="18" t="s">
+        <v>389</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>390</v>
+      </c>
+      <c r="L26" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="M26" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="N26" s="4" t="s">
         <v>180</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="H26" t="s">
-        <v>325</v>
-      </c>
-      <c r="I26" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="J26" t="s">
-        <v>356</v>
-      </c>
-      <c r="L26" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="N26" s="4" t="s">
-        <v>186</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="14" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="D27" s="15" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="G27" s="15" t="s">
-        <v>387</v>
+        <v>377</v>
       </c>
       <c r="H27" s="15" t="s">
-        <v>390</v>
+        <v>380</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>388</v>
+        <v>378</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="M27" s="15" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P27" s="4"/>
       <c r="Q27" s="4"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="H28" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="I28" s="8" t="s">
-        <v>304</v>
+        <v>296</v>
       </c>
       <c r="J28" t="s">
-        <v>357</v>
+        <v>347</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P28" s="4"/>
       <c r="Q28" s="4"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="C29" t="s">
+        <v>186</v>
+      </c>
+      <c r="D29" t="s">
+        <v>187</v>
+      </c>
+      <c r="E29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="H29" t="s">
+        <v>318</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="J29" t="s">
+        <v>348</v>
+      </c>
+      <c r="L29" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="M29" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="C29" t="s">
-        <v>192</v>
-      </c>
-      <c r="D29" t="s">
-        <v>193</v>
-      </c>
-      <c r="E29" t="s">
-        <v>194</v>
-      </c>
-      <c r="G29" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="H29" t="s">
-        <v>327</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="J29" t="s">
-        <v>358</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="M29" s="4" t="s">
-        <v>196</v>
-      </c>
       <c r="N29" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="H30" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="J30" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P31" s="4"/>
       <c r="Q31" s="4"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="C32" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="E32" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H32" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="I32" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="J32" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="C33" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="D33" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="E33" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="H33" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="I33" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="J33" t="s">
-        <v>362</v>
+        <v>352</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="H34" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="I34" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="J34" t="s">
-        <v>363</v>
+        <v>353</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C36" t="s">
+        <v>215</v>
+      </c>
+      <c r="D36" t="s">
+        <v>216</v>
+      </c>
+      <c r="E36" t="s">
+        <v>217</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="H36" t="s">
+        <v>325</v>
+      </c>
+      <c r="I36" t="s">
+        <v>266</v>
+      </c>
+      <c r="J36" t="s">
+        <v>355</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="M36" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C36" t="s">
-        <v>221</v>
-      </c>
-      <c r="D36" t="s">
-        <v>222</v>
-      </c>
-      <c r="E36" t="s">
-        <v>223</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="H36" t="s">
-        <v>334</v>
-      </c>
-      <c r="I36" t="s">
-        <v>274</v>
-      </c>
-      <c r="J36" t="s">
-        <v>365</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="M36" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="N36" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P36" s="4"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G37" s="8" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H37" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="J37" t="s">
-        <v>366</v>
+        <v>356</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="P37" s="4"/>
       <c r="Q37" s="4"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="E38" s="8" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="H38" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="I38" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="J38" t="s">
-        <v>367</v>
+        <v>357</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
-        <v>368</v>
+        <v>358</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="E39" s="11" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="G39" s="11" t="s">
-        <v>369</v>
+        <v>359</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>370</v>
+        <v>360</v>
       </c>
       <c r="I39" s="9" t="s">
-        <v>372</v>
+        <v>362</v>
       </c>
       <c r="J39" s="11" t="s">
-        <v>373</v>
+        <v>363</v>
       </c>
       <c r="L39" s="4" t="s">
         <v>17</v>
@@ -3295,31 +3301,31 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
-        <v>374</v>
+        <v>364</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>376</v>
+        <v>366</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="L40" s="4" t="s">
         <v>49</v>
@@ -3333,31 +3339,31 @@
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="10" t="s">
-        <v>375</v>
+        <v>365</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="L41" s="4" t="s">
         <v>133</v>

</xml_diff>

<commit_message>
replace duplicate properties for metadata in daschland ontology with properties from project_metadata ontology
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01245E07-5910-8340-8954-DB4E1658C0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97253E3-DC9B-3E47-AF83-AB3A83AB1D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$36</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="355">
   <si>
     <t>name</t>
   </si>
@@ -436,30 +436,6 @@
     <t>hasValue, schema:name</t>
   </si>
   <si>
-    <t>hasFileSize</t>
-  </si>
-  <si>
-    <t>File Size (Mb)</t>
-  </si>
-  <si>
-    <t>Dateigrösse (Mb)</t>
-  </si>
-  <si>
-    <t>Taille du fichier (Mb)</t>
-  </si>
-  <si>
-    <t>Dimensioni del file (Mb)</t>
-  </si>
-  <si>
-    <t>Size of the file in Mb</t>
-  </si>
-  <si>
-    <t>hasValue, schema:size</t>
-  </si>
-  <si>
-    <t>DecimalValue</t>
-  </si>
-  <si>
     <t>hasFullText</t>
   </si>
   <si>
@@ -643,30 +619,6 @@
     <t>seqnum, schema:position</t>
   </si>
   <si>
-    <t>hasTimeStamp</t>
-  </si>
-  <si>
-    <t>Time Stamp</t>
-  </si>
-  <si>
-    <t>Zeitstempel</t>
-  </si>
-  <si>
-    <t>Horodatage</t>
-  </si>
-  <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
-    <t>hasValue, schema:dateCreated</t>
-  </si>
-  <si>
-    <t>TimeValue</t>
-  </si>
-  <si>
-    <t>TimeStamp</t>
-  </si>
-  <si>
     <t>hasUrl</t>
   </si>
   <si>
@@ -865,9 +817,6 @@
     <t>Sequence number used for compound object</t>
   </si>
   <si>
-    <t>Time stamp</t>
-  </si>
-  <si>
     <t>URL leading to an external page with more information</t>
   </si>
   <si>
@@ -925,9 +874,6 @@
     <t>Nom du fichier original</t>
   </si>
   <si>
-    <t>Taille du fichier en Mo</t>
-  </si>
-  <si>
     <t>Texte en anglais</t>
   </si>
   <si>
@@ -1090,9 +1036,6 @@
     <t>Name der Originaldatei</t>
   </si>
   <si>
-    <t>Dateigröße in MB</t>
-  </si>
-  <si>
     <t>Text in englischer Sprache</t>
   </si>
   <si>
@@ -1177,9 +1120,6 @@
     <t>Nome del file originale</t>
   </si>
   <si>
-    <t>Dimensione del file in Mb</t>
-  </si>
-  <si>
     <t>Testo in inglese</t>
   </si>
   <si>
@@ -1207,9 +1147,6 @@
     <t>Numero di sequenza utilizzato per oggetti composti</t>
   </si>
   <si>
-    <t>Data e ora</t>
-  </si>
-  <si>
     <t>URL che rimanda a una pagina esterna con ulteriori informazioni</t>
   </si>
   <si>
@@ -1249,52 +1186,7 @@
     <t>link interno a Copertina/e del libro</t>
   </si>
   <si>
-    <t>hasAuthorshipResource</t>
-  </si>
-  <si>
-    <t>Author of the resource</t>
-  </si>
-  <si>
-    <t>Autor der Resource</t>
-  </si>
-  <si>
     <t>Auteur·rice</t>
-  </si>
-  <si>
-    <t>Auteur·rice de la ressource</t>
-  </si>
-  <si>
-    <t>Autore della risorsa</t>
-  </si>
-  <si>
-    <t>hasCopyrightResource</t>
-  </si>
-  <si>
-    <t>hasLicenseResource</t>
-  </si>
-  <si>
-    <t>Copyright of the resource</t>
-  </si>
-  <si>
-    <t>License of the resource</t>
-  </si>
-  <si>
-    <t>Lizenz der Resource</t>
-  </si>
-  <si>
-    <t>Urheberrecht der Resource</t>
-  </si>
-  <si>
-    <t>Licence de la ressource</t>
-  </si>
-  <si>
-    <t>Droits d'auteur de la ressource</t>
-  </si>
-  <si>
-    <t>Copyright della risorsa</t>
-  </si>
-  <si>
-    <t>Licenza della risorsa</t>
   </si>
   <si>
     <t>default_permissions_overrule</t>
@@ -1352,19 +1244,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1451,13 +1336,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.199999999999999"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1491,20 +1369,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1726,11 +1602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q917"/>
+  <dimension ref="A1:Q912"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1801,22 +1677,22 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>374</v>
+      <c r="P1" s="10" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1825,13 +1701,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
@@ -1863,13 +1739,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="I3" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="J3" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
@@ -1877,8 +1753,8 @@
       <c r="M3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>381</v>
+      <c r="N3" s="14" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1901,10 +1777,10 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="I4" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1980,13 +1856,13 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="I6" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="J6" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -2020,7 +1896,7 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -2062,7 +1938,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>62</v>
@@ -2099,13 +1975,13 @@
         <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
@@ -2116,8 +1992,8 @@
       <c r="N9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="13" t="s">
-        <v>375</v>
+      <c r="P9" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
@@ -2141,13 +2017,13 @@
         <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="J10" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
@@ -2182,13 +2058,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="J11" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
@@ -2221,179 +2097,182 @@
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="I12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="J12" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="H13" t="s">
+        <v>288</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" t="s">
+        <v>316</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G13" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" t="s">
-        <v>306</v>
-      </c>
-      <c r="I13" t="s">
-        <v>251</v>
-      </c>
-      <c r="J13" t="s">
-        <v>335</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="D14" t="s">
         <v>103</v>
       </c>
-      <c r="C14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>103</v>
+      <c r="E14" t="s">
+        <v>104</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H14" t="s">
-        <v>307</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>269</v>
+        <v>289</v>
+      </c>
+      <c r="I14" t="s">
+        <v>234</v>
       </c>
       <c r="J14" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
+        <v>290</v>
+      </c>
+      <c r="I15" t="s">
+        <v>235</v>
+      </c>
+      <c r="J15" t="s">
+        <v>318</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" t="s">
-        <v>308</v>
-      </c>
-      <c r="I15" t="s">
-        <v>252</v>
-      </c>
-      <c r="J15" t="s">
-        <v>337</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="M15" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="G16" t="s">
         <v>116</v>
       </c>
-      <c r="C16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" t="s">
+        <v>291</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="J16" t="s">
+        <v>319</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H16" t="s">
-        <v>309</v>
-      </c>
-      <c r="I16" t="s">
-        <v>253</v>
-      </c>
-      <c r="J16" t="s">
-        <v>338</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -2402,26 +2281,26 @@
       <c r="B17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>122</v>
       </c>
       <c r="E17" t="s">
         <v>123</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>310</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>270</v>
+        <v>292</v>
+      </c>
+      <c r="I17" t="s">
+        <v>236</v>
       </c>
       <c r="J17" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
@@ -2435,6 +2314,8 @@
       <c r="O17" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
@@ -2444,619 +2325,612 @@
         <v>128</v>
       </c>
       <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>130</v>
       </c>
-      <c r="E18" t="s">
-        <v>131</v>
-      </c>
       <c r="G18" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H18" t="s">
-        <v>311</v>
-      </c>
-      <c r="I18" t="s">
-        <v>254</v>
+        <v>128</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="J18" t="s">
-        <v>340</v>
+        <v>130</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" t="s">
         <v>135</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" t="s">
-        <v>138</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>136</v>
       </c>
       <c r="H19" t="s">
-        <v>136</v>
-      </c>
-      <c r="I19" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="I19" t="s">
+        <v>237</v>
+      </c>
+      <c r="J19" t="s">
+        <v>321</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J19" t="s">
-        <v>138</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P19" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="P19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" t="s">
         <v>140</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>141</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>142</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20" t="s">
+        <v>238</v>
+      </c>
+      <c r="J20" t="s">
+        <v>322</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="M20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H20" t="s">
-        <v>312</v>
-      </c>
-      <c r="I20" t="s">
-        <v>255</v>
-      </c>
-      <c r="J20" t="s">
-        <v>341</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" t="s">
+        <v>295</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>323</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="H21" t="s">
-        <v>313</v>
-      </c>
-      <c r="I21" t="s">
-        <v>256</v>
-      </c>
-      <c r="J21" t="s">
-        <v>342</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="M21" s="4" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22" t="s">
+        <v>296</v>
+      </c>
+      <c r="I22" t="s">
+        <v>240</v>
+      </c>
+      <c r="J22" t="s">
+        <v>324</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C22" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" t="s">
-        <v>154</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="H22" t="s">
-        <v>314</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="J22" t="s">
-        <v>343</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" t="s">
         <v>157</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>158</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>159</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H23" t="s">
+        <v>297</v>
+      </c>
+      <c r="I23" t="s">
+        <v>241</v>
+      </c>
+      <c r="J23" t="s">
+        <v>325</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="H23" t="s">
-        <v>158</v>
-      </c>
-      <c r="I23" t="s">
-        <v>159</v>
-      </c>
-      <c r="J23" t="s">
-        <v>344</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="N23" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="N24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" t="s">
-        <v>168</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H24" t="s">
-        <v>315</v>
-      </c>
-      <c r="I24" t="s">
-        <v>258</v>
-      </c>
-      <c r="J24" t="s">
-        <v>345</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" t="s">
-        <v>175</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="H25" t="s">
-        <v>316</v>
-      </c>
-      <c r="I25" t="s">
-        <v>259</v>
-      </c>
-      <c r="J25" t="s">
-        <v>346</v>
+      <c r="A25" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>343</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>178</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>382</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>390</v>
+      <c r="A26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="H26" t="s">
+        <v>298</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J26" t="s">
+        <v>326</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M26" s="18" t="s">
-        <v>190</v>
+        <v>166</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>379</v>
+      <c r="A27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H27" t="s">
+        <v>299</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="J27" t="s">
+        <v>327</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M27" s="15" t="s">
-        <v>196</v>
+        <v>173</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>294</v>
+        <v>216</v>
       </c>
       <c r="H28" t="s">
-        <v>317</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>296</v>
+        <v>300</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="J28" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C29" t="s">
-        <v>186</v>
-      </c>
-      <c r="D29" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" t="s">
-        <v>188</v>
+        <v>178</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="H29" t="s">
-        <v>318</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="J29" t="s">
-        <v>348</v>
+        <v>217</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>277</v>
+        <v>181</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" t="s">
+        <v>183</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>289</v>
+        <v>184</v>
+      </c>
+      <c r="E30" t="s">
+        <v>185</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H30" t="s">
-        <v>319</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>260</v>
+        <v>302</v>
+      </c>
+      <c r="I30" t="s">
+        <v>244</v>
       </c>
       <c r="J30" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>293</v>
+        <v>186</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" t="s">
+        <v>190</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>350</v>
+        <v>224</v>
+      </c>
+      <c r="H31" t="s">
+        <v>303</v>
+      </c>
+      <c r="I31" t="s">
+        <v>245</v>
+      </c>
+      <c r="J31" t="s">
+        <v>331</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C32" t="s">
-        <v>199</v>
+        <v>191</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" t="s">
-        <v>201</v>
+        <v>265</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="H32" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="I32" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="J32" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33" t="s">
-        <v>206</v>
+        <v>194</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>273</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="H33" t="s">
-        <v>322</v>
-      </c>
-      <c r="I33" t="s">
-        <v>263</v>
-      </c>
-      <c r="J33" t="s">
-        <v>352</v>
+        <v>219</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>195</v>
@@ -3065,319 +2939,131 @@
         <v>196</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>290</v>
+        <v>198</v>
+      </c>
+      <c r="C34" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" t="s">
+        <v>201</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="H34" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="I34" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="J34" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P34" s="4"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>324</v>
+        <v>221</v>
+      </c>
+      <c r="H35" t="s">
+        <v>307</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>354</v>
+        <v>249</v>
+      </c>
+      <c r="J35" t="s">
+        <v>335</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C36" t="s">
-        <v>215</v>
-      </c>
-      <c r="D36" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36" t="s">
-        <v>217</v>
+        <v>257</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="H36" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="I36" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="J36" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P36" s="4"/>
+        <v>164</v>
+      </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="H37" t="s">
-        <v>326</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="J37" t="s">
-        <v>356</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-    </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="H38" t="s">
-        <v>327</v>
-      </c>
-      <c r="I38" t="s">
-        <v>268</v>
-      </c>
-      <c r="J38" t="s">
-        <v>357</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="J41" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4249,13 +3935,8 @@
     <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:Q38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="property-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="property-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>

<commit_message>
replace duplicate properties for metadata in daschland ontology with properties from project_metadata ontology (#71)
</commit_message>
<xml_diff>
--- a/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
+++ b/daschland_ontology/daschland (Alice in DaSCHland)/properties.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noemivillars-amberg/Documents/daschland-scripts/daschland_ontology/daschland (Alice in DaSCHland)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01245E07-5910-8340-8954-DB4E1658C0D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D97253E3-DC9B-3E47-AF83-AB3A83AB1D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3800" yWindow="500" windowWidth="68740" windowHeight="30240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,9 +16,9 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Q$36</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="391">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="355">
   <si>
     <t>name</t>
   </si>
@@ -436,30 +436,6 @@
     <t>hasValue, schema:name</t>
   </si>
   <si>
-    <t>hasFileSize</t>
-  </si>
-  <si>
-    <t>File Size (Mb)</t>
-  </si>
-  <si>
-    <t>Dateigrösse (Mb)</t>
-  </si>
-  <si>
-    <t>Taille du fichier (Mb)</t>
-  </si>
-  <si>
-    <t>Dimensioni del file (Mb)</t>
-  </si>
-  <si>
-    <t>Size of the file in Mb</t>
-  </si>
-  <si>
-    <t>hasValue, schema:size</t>
-  </si>
-  <si>
-    <t>DecimalValue</t>
-  </si>
-  <si>
     <t>hasFullText</t>
   </si>
   <si>
@@ -643,30 +619,6 @@
     <t>seqnum, schema:position</t>
   </si>
   <si>
-    <t>hasTimeStamp</t>
-  </si>
-  <si>
-    <t>Time Stamp</t>
-  </si>
-  <si>
-    <t>Zeitstempel</t>
-  </si>
-  <si>
-    <t>Horodatage</t>
-  </si>
-  <si>
-    <t>Timestamp</t>
-  </si>
-  <si>
-    <t>hasValue, schema:dateCreated</t>
-  </si>
-  <si>
-    <t>TimeValue</t>
-  </si>
-  <si>
-    <t>TimeStamp</t>
-  </si>
-  <si>
     <t>hasUrl</t>
   </si>
   <si>
@@ -865,9 +817,6 @@
     <t>Sequence number used for compound object</t>
   </si>
   <si>
-    <t>Time stamp</t>
-  </si>
-  <si>
     <t>URL leading to an external page with more information</t>
   </si>
   <si>
@@ -925,9 +874,6 @@
     <t>Nom du fichier original</t>
   </si>
   <si>
-    <t>Taille du fichier en Mo</t>
-  </si>
-  <si>
     <t>Texte en anglais</t>
   </si>
   <si>
@@ -1090,9 +1036,6 @@
     <t>Name der Originaldatei</t>
   </si>
   <si>
-    <t>Dateigröße in MB</t>
-  </si>
-  <si>
     <t>Text in englischer Sprache</t>
   </si>
   <si>
@@ -1177,9 +1120,6 @@
     <t>Nome del file originale</t>
   </si>
   <si>
-    <t>Dimensione del file in Mb</t>
-  </si>
-  <si>
     <t>Testo in inglese</t>
   </si>
   <si>
@@ -1207,9 +1147,6 @@
     <t>Numero di sequenza utilizzato per oggetti composti</t>
   </si>
   <si>
-    <t>Data e ora</t>
-  </si>
-  <si>
     <t>URL che rimanda a una pagina esterna con ulteriori informazioni</t>
   </si>
   <si>
@@ -1249,52 +1186,7 @@
     <t>link interno a Copertina/e del libro</t>
   </si>
   <si>
-    <t>hasAuthorshipResource</t>
-  </si>
-  <si>
-    <t>Author of the resource</t>
-  </si>
-  <si>
-    <t>Autor der Resource</t>
-  </si>
-  <si>
     <t>Auteur·rice</t>
-  </si>
-  <si>
-    <t>Auteur·rice de la ressource</t>
-  </si>
-  <si>
-    <t>Autore della risorsa</t>
-  </si>
-  <si>
-    <t>hasCopyrightResource</t>
-  </si>
-  <si>
-    <t>hasLicenseResource</t>
-  </si>
-  <si>
-    <t>Copyright of the resource</t>
-  </si>
-  <si>
-    <t>License of the resource</t>
-  </si>
-  <si>
-    <t>Lizenz der Resource</t>
-  </si>
-  <si>
-    <t>Urheberrecht der Resource</t>
-  </si>
-  <si>
-    <t>Licence de la ressource</t>
-  </si>
-  <si>
-    <t>Droits d'auteur de la ressource</t>
-  </si>
-  <si>
-    <t>Copyright della risorsa</t>
-  </si>
-  <si>
-    <t>Licenza della risorsa</t>
   </si>
   <si>
     <t>default_permissions_overrule</t>
@@ -1352,19 +1244,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1451,13 +1336,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF333333"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10.199999999999999"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -1491,20 +1369,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1726,11 +1602,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q917"/>
+  <dimension ref="A1:Q912"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" zoomScaleNormal="172" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1801,22 +1677,22 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="12" t="s">
-        <v>374</v>
+      <c r="P1" s="10" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>361</v>
+        <v>337</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>15</v>
@@ -1825,13 +1701,13 @@
         <v>16</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>242</v>
+        <v>225</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>328</v>
+        <v>309</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>17</v>
@@ -1863,13 +1739,13 @@
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>298</v>
+        <v>280</v>
       </c>
       <c r="I3" t="s">
-        <v>243</v>
+        <v>226</v>
       </c>
       <c r="J3" t="s">
-        <v>329</v>
+        <v>310</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>26</v>
@@ -1877,8 +1753,8 @@
       <c r="M3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="N3" s="16" t="s">
-        <v>381</v>
+      <c r="N3" s="14" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1901,10 +1777,10 @@
         <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>299</v>
+        <v>281</v>
       </c>
       <c r="I4" t="s">
-        <v>244</v>
+        <v>227</v>
       </c>
       <c r="J4" t="s">
         <v>32</v>
@@ -1980,13 +1856,13 @@
         <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="I6" t="s">
-        <v>245</v>
+        <v>228</v>
       </c>
       <c r="J6" t="s">
-        <v>330</v>
+        <v>311</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>49</v>
@@ -2020,7 +1896,7 @@
         <v>55</v>
       </c>
       <c r="H7" t="s">
-        <v>301</v>
+        <v>283</v>
       </c>
       <c r="I7" t="s">
         <v>53</v>
@@ -2062,7 +1938,7 @@
         <v>61</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>246</v>
+        <v>229</v>
       </c>
       <c r="J8" s="4" t="s">
         <v>62</v>
@@ -2099,13 +1975,13 @@
         <v>69</v>
       </c>
       <c r="H9" t="s">
-        <v>302</v>
+        <v>284</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>247</v>
+        <v>230</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>331</v>
+        <v>312</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>63</v>
@@ -2116,8 +1992,8 @@
       <c r="N9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="P9" s="13" t="s">
-        <v>375</v>
+      <c r="P9" s="11" t="s">
+        <v>339</v>
       </c>
       <c r="Q9" s="4"/>
     </row>
@@ -2141,13 +2017,13 @@
         <v>75</v>
       </c>
       <c r="H10" t="s">
-        <v>303</v>
+        <v>285</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>248</v>
+        <v>231</v>
       </c>
       <c r="J10" t="s">
-        <v>332</v>
+        <v>313</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>76</v>
@@ -2182,13 +2058,13 @@
         <v>85</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>304</v>
+        <v>286</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>249</v>
+        <v>232</v>
       </c>
       <c r="J11" t="s">
-        <v>333</v>
+        <v>314</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>86</v>
@@ -2221,179 +2097,182 @@
         <v>92</v>
       </c>
       <c r="H12" t="s">
-        <v>305</v>
+        <v>287</v>
       </c>
       <c r="I12" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="J12" t="s">
-        <v>334</v>
+        <v>315</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>93</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>94</v>
+        <v>18</v>
       </c>
       <c r="N12" s="4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="C13" t="s">
+        <v>95</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="G13" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="H13" t="s">
+        <v>288</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="J13" t="s">
+        <v>316</v>
+      </c>
+      <c r="L13" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="M13" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="N13" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G13" t="s">
-        <v>100</v>
-      </c>
-      <c r="H13" t="s">
-        <v>306</v>
-      </c>
-      <c r="I13" t="s">
-        <v>251</v>
-      </c>
-      <c r="J13" t="s">
-        <v>335</v>
-      </c>
-      <c r="L13" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="M13" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N13" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="D14" t="s">
         <v>103</v>
       </c>
-      <c r="C14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>103</v>
+      <c r="E14" t="s">
+        <v>104</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H14" t="s">
-        <v>307</v>
-      </c>
-      <c r="I14" s="8" t="s">
-        <v>269</v>
+        <v>289</v>
+      </c>
+      <c r="I14" t="s">
+        <v>234</v>
       </c>
       <c r="J14" t="s">
-        <v>336</v>
+        <v>317</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
       <c r="N14" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>108</v>
+      </c>
+      <c r="E15" t="s">
+        <v>108</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C15" t="s">
+      <c r="H15" t="s">
+        <v>290</v>
+      </c>
+      <c r="I15" t="s">
+        <v>235</v>
+      </c>
+      <c r="J15" t="s">
+        <v>318</v>
+      </c>
+      <c r="L15" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D15" t="s">
-        <v>111</v>
-      </c>
-      <c r="E15" t="s">
-        <v>112</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="H15" t="s">
-        <v>308</v>
-      </c>
-      <c r="I15" t="s">
-        <v>252</v>
-      </c>
-      <c r="J15" t="s">
-        <v>337</v>
-      </c>
-      <c r="L15" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="M15" s="4" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="N15" s="4" t="s">
         <v>19</v>
       </c>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="4"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="G16" t="s">
         <v>116</v>
       </c>
-      <c r="C16" t="s">
-        <v>116</v>
-      </c>
-      <c r="D16" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" t="s">
-        <v>116</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="H16" t="s">
+        <v>291</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="J16" t="s">
+        <v>319</v>
+      </c>
+      <c r="L16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="H16" t="s">
-        <v>309</v>
-      </c>
-      <c r="I16" t="s">
-        <v>253</v>
-      </c>
-      <c r="J16" t="s">
-        <v>338</v>
-      </c>
-      <c r="L16" s="4" t="s">
+      <c r="M16" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O16" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="M16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="4"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
@@ -2402,26 +2281,26 @@
       <c r="B17" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C17" t="s">
         <v>121</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" t="s">
         <v>122</v>
       </c>
       <c r="E17" t="s">
         <v>123</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="4" t="s">
         <v>124</v>
       </c>
       <c r="H17" t="s">
-        <v>310</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>270</v>
+        <v>292</v>
+      </c>
+      <c r="I17" t="s">
+        <v>236</v>
       </c>
       <c r="J17" t="s">
-        <v>339</v>
+        <v>320</v>
       </c>
       <c r="L17" s="4" t="s">
         <v>125</v>
@@ -2435,6 +2314,8 @@
       <c r="O17" s="4" t="s">
         <v>126</v>
       </c>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
@@ -2444,619 +2325,612 @@
         <v>128</v>
       </c>
       <c r="C18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>130</v>
       </c>
-      <c r="E18" t="s">
-        <v>131</v>
-      </c>
       <c r="G18" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H18" t="s">
-        <v>311</v>
-      </c>
-      <c r="I18" t="s">
-        <v>254</v>
+        <v>128</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>129</v>
       </c>
       <c r="J18" t="s">
-        <v>340</v>
+        <v>130</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>133</v>
+        <v>86</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="N18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O18" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
+        <v>19</v>
+      </c>
+      <c r="P18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C19" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" t="s">
+        <v>134</v>
+      </c>
+      <c r="E19" t="s">
         <v>135</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C19" t="s">
-        <v>136</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E19" t="s">
-        <v>138</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>136</v>
       </c>
       <c r="H19" t="s">
-        <v>136</v>
-      </c>
-      <c r="I19" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="I19" t="s">
+        <v>237</v>
+      </c>
+      <c r="J19" t="s">
+        <v>321</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="J19" t="s">
-        <v>138</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>86</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P19" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="P19" s="4"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="C20" t="s">
         <v>140</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>141</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>142</v>
       </c>
-      <c r="E20" t="s">
+      <c r="G20" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="H20" t="s">
+        <v>294</v>
+      </c>
+      <c r="I20" t="s">
+        <v>238</v>
+      </c>
+      <c r="J20" t="s">
+        <v>322</v>
+      </c>
+      <c r="L20" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="M20" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="O20" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="H20" t="s">
-        <v>312</v>
-      </c>
-      <c r="I20" t="s">
-        <v>255</v>
-      </c>
-      <c r="J20" t="s">
-        <v>341</v>
-      </c>
-      <c r="L20" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="M20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N20" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B21" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="C21" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" t="s">
+        <v>295</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="J21" t="s">
+        <v>323</v>
+      </c>
+      <c r="L21" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="C21" t="s">
-        <v>148</v>
-      </c>
-      <c r="D21" t="s">
-        <v>149</v>
-      </c>
-      <c r="E21" t="s">
-        <v>150</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>228</v>
-      </c>
-      <c r="H21" t="s">
-        <v>313</v>
-      </c>
-      <c r="I21" t="s">
-        <v>256</v>
-      </c>
-      <c r="J21" t="s">
-        <v>342</v>
-      </c>
-      <c r="L21" s="4" t="s">
-        <v>151</v>
-      </c>
       <c r="M21" s="4" t="s">
-        <v>77</v>
+        <v>35</v>
       </c>
       <c r="N21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O21" s="4" t="s">
-        <v>152</v>
+        <v>19</v>
       </c>
       <c r="P21" s="4"/>
       <c r="Q21" s="4"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E22" t="s">
+        <v>152</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="H22" t="s">
+        <v>296</v>
+      </c>
+      <c r="I22" t="s">
+        <v>240</v>
+      </c>
+      <c r="J22" t="s">
+        <v>324</v>
+      </c>
+      <c r="L22" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="M22" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C22" t="s">
-        <v>154</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="E22" t="s">
-        <v>154</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="H22" t="s">
-        <v>314</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="J22" t="s">
-        <v>343</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>35</v>
       </c>
       <c r="N22" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="P22" s="4"/>
-      <c r="Q22" s="4"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" t="s">
         <v>157</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>158</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>159</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="H23" t="s">
+        <v>297</v>
+      </c>
+      <c r="I23" t="s">
+        <v>241</v>
+      </c>
+      <c r="J23" t="s">
+        <v>325</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>230</v>
-      </c>
-      <c r="H23" t="s">
-        <v>158</v>
-      </c>
-      <c r="I23" t="s">
-        <v>159</v>
-      </c>
-      <c r="J23" t="s">
-        <v>344</v>
-      </c>
-      <c r="L23" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="M23" s="4" t="s">
+      <c r="N23" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="N23" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="P23" s="4"/>
-      <c r="Q23" s="4"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="15" t="s">
+        <v>346</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>347</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>352</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>353</v>
+      </c>
+      <c r="J24" s="16" t="s">
+        <v>354</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="N24" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="D24" t="s">
-        <v>167</v>
-      </c>
-      <c r="E24" t="s">
-        <v>168</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>231</v>
-      </c>
-      <c r="H24" t="s">
-        <v>315</v>
-      </c>
-      <c r="I24" t="s">
-        <v>258</v>
-      </c>
-      <c r="J24" t="s">
-        <v>345</v>
-      </c>
-      <c r="L24" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>19</v>
-      </c>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C25" t="s">
-        <v>173</v>
-      </c>
-      <c r="D25" t="s">
-        <v>174</v>
-      </c>
-      <c r="E25" t="s">
-        <v>175</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="H25" t="s">
-        <v>316</v>
-      </c>
-      <c r="I25" t="s">
-        <v>259</v>
-      </c>
-      <c r="J25" t="s">
-        <v>346</v>
+      <c r="A25" s="12" t="s">
+        <v>340</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>342</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>343</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>177</v>
+        <v>163</v>
+      </c>
+      <c r="M25" s="13" t="s">
+        <v>180</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>178</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="17" t="s">
-        <v>382</v>
-      </c>
-      <c r="B26" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>384</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>383</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>386</v>
-      </c>
-      <c r="G26" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="H26" s="18" t="s">
-        <v>388</v>
-      </c>
-      <c r="I26" s="18" t="s">
-        <v>389</v>
-      </c>
-      <c r="J26" s="18" t="s">
-        <v>390</v>
+      <c r="A26" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="G26" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="H26" t="s">
+        <v>298</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="J26" t="s">
+        <v>326</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M26" s="18" t="s">
-        <v>190</v>
+        <v>166</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>167</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
-        <v>376</v>
-      </c>
-      <c r="B27" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>377</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>380</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>378</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>379</v>
+      <c r="A27" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" t="s">
+        <v>170</v>
+      </c>
+      <c r="D27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E27" t="s">
+        <v>172</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H27" t="s">
+        <v>299</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="J27" t="s">
+        <v>327</v>
       </c>
       <c r="L27" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M27" s="15" t="s">
-        <v>196</v>
+        <v>173</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>174</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>276</v>
+        <v>259</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>294</v>
+        <v>216</v>
       </c>
       <c r="H28" t="s">
-        <v>317</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>296</v>
+        <v>300</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>242</v>
       </c>
       <c r="J28" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P28" s="4"/>
-      <c r="Q28" s="4"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="C29" t="s">
-        <v>186</v>
-      </c>
-      <c r="D29" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" t="s">
-        <v>188</v>
+        <v>178</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>275</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>271</v>
-      </c>
-      <c r="H29" t="s">
-        <v>318</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>295</v>
-      </c>
-      <c r="J29" t="s">
-        <v>348</v>
+        <v>217</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>329</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>277</v>
+        <v>181</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" t="s">
+        <v>183</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>272</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>289</v>
+        <v>184</v>
+      </c>
+      <c r="E30" t="s">
+        <v>185</v>
       </c>
       <c r="G30" s="8" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="H30" t="s">
-        <v>319</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>260</v>
+        <v>302</v>
+      </c>
+      <c r="I30" t="s">
+        <v>244</v>
       </c>
       <c r="J30" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>273</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>278</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>293</v>
+        <v>186</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="C31" t="s">
+        <v>188</v>
+      </c>
+      <c r="D31" t="s">
+        <v>189</v>
+      </c>
+      <c r="E31" t="s">
+        <v>190</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>320</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>350</v>
+        <v>224</v>
+      </c>
+      <c r="H31" t="s">
+        <v>303</v>
+      </c>
+      <c r="I31" t="s">
+        <v>245</v>
+      </c>
+      <c r="J31" t="s">
+        <v>331</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="N31" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P31" s="4"/>
-      <c r="Q31" s="4"/>
+        <v>164</v>
+      </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="C32" t="s">
-        <v>199</v>
+        <v>191</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>261</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>200</v>
-      </c>
-      <c r="E32" t="s">
-        <v>201</v>
+        <v>265</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>272</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="H32" t="s">
-        <v>321</v>
+        <v>304</v>
       </c>
       <c r="I32" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="J32" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="N32" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="C33" t="s">
-        <v>204</v>
-      </c>
-      <c r="D33" t="s">
-        <v>205</v>
-      </c>
-      <c r="E33" t="s">
-        <v>206</v>
+        <v>194</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>273</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="H33" t="s">
-        <v>322</v>
-      </c>
-      <c r="I33" t="s">
-        <v>263</v>
-      </c>
-      <c r="J33" t="s">
-        <v>352</v>
+        <v>219</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>333</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>195</v>
@@ -3065,319 +2939,131 @@
         <v>196</v>
       </c>
       <c r="N33" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>284</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>279</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>283</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>290</v>
+        <v>198</v>
+      </c>
+      <c r="C34" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" t="s">
+        <v>200</v>
+      </c>
+      <c r="E34" t="s">
+        <v>201</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="H34" t="s">
-        <v>323</v>
+        <v>306</v>
       </c>
       <c r="I34" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="J34" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="L34" s="4" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>209</v>
+        <v>203</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P34" s="4"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>285</v>
+        <v>256</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>280</v>
+        <v>256</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>286</v>
+        <v>269</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>291</v>
+        <v>256</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>324</v>
+        <v>221</v>
+      </c>
+      <c r="H35" t="s">
+        <v>307</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>354</v>
+        <v>249</v>
+      </c>
+      <c r="J35" t="s">
+        <v>335</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C36" t="s">
-        <v>215</v>
-      </c>
-      <c r="D36" t="s">
-        <v>216</v>
-      </c>
-      <c r="E36" t="s">
-        <v>217</v>
+        <v>257</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>274</v>
       </c>
       <c r="G36" s="8" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
       <c r="H36" t="s">
-        <v>325</v>
+        <v>308</v>
       </c>
       <c r="I36" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="J36" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P36" s="4"/>
+        <v>164</v>
+      </c>
     </row>
-    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>287</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>274</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="H37" t="s">
-        <v>326</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="J37" t="s">
-        <v>356</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="M37" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="N37" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="P37" s="4"/>
-      <c r="Q37" s="4"/>
-    </row>
-    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>288</v>
-      </c>
-      <c r="E38" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="G38" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="H38" t="s">
-        <v>327</v>
-      </c>
-      <c r="I38" t="s">
-        <v>268</v>
-      </c>
-      <c r="J38" t="s">
-        <v>357</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="N38" s="4" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="B39" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="E39" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>359</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="I39" s="9" t="s">
-        <v>362</v>
-      </c>
-      <c r="J39" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="L39" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M39" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N39" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="10" t="s">
-        <v>364</v>
-      </c>
-      <c r="B40" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="C40" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="E40" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>366</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>369</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="J40" s="11" t="s">
-        <v>372</v>
-      </c>
-      <c r="L40" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="M40" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="B41" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="C41" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>367</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>368</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>370</v>
-      </c>
-      <c r="J41" s="11" t="s">
-        <v>373</v>
-      </c>
-      <c r="L41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="M41" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="N41" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="O41" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
+    <row r="37" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="43" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="44" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4249,13 +3935,8 @@
     <row r="910" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="911" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="912" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="913" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="914" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="915" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="916" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="917" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:Q38" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q36" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" location="property-name" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B1" r:id="rId2" location="property-labels" xr:uid="{00000000-0004-0000-0000-000001000000}"/>

</xml_diff>